<commit_message>
fixed Scen_IEAcosts_TRA, should sync with VEDA now
</commit_message>
<xml_diff>
--- a/suppxls/Scen_IEAcosts_TRA.xlsx
+++ b/suppxls/Scen_IEAcosts_TRA.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SATIMGE_Veda\suppxls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38F7E041-72A8-42A9-81E7-6B1C4BBDBF83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{899A7558-5E40-4C2B-BFED-E283E4ECFEA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{E2E76818-39F4-4BBE-93AA-8C71FE1D5983}"/>
-    <workbookView xWindow="2880" yWindow="0" windowWidth="21315" windowHeight="12510" activeTab="2" xr2:uid="{2CAB5348-3A5C-453D-8E79-FBBD2C206FCF}"/>
+    <workbookView xWindow="735" yWindow="735" windowWidth="28800" windowHeight="15480" activeTab="1" xr2:uid="{E2E76818-39F4-4BBE-93AA-8C71FE1D5983}"/>
+    <workbookView xWindow="1080" yWindow="1080" windowWidth="28800" windowHeight="15480" activeTab="2" xr2:uid="{2CAB5348-3A5C-453D-8E79-FBBD2C206FCF}"/>
   </bookViews>
   <sheets>
     <sheet name="INVCOST" sheetId="13" r:id="rId1"/>
@@ -51,7 +51,7 @@
     <definedName name="_AtRisk_SimSetting_StdRecalcWithoutRiskStatic" hidden="1">0</definedName>
     <definedName name="_AtRisk_SimSetting_StdRecalcWithoutRiskStaticPercentile" hidden="1">0.5</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">CostProjections!$A$10:$M$92</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">FIXOM!$A$6:$O$83</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">FIXOM!$A$6:$I$83</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">INVCOST!$A$6:$O$83</definedName>
     <definedName name="base.year">[1]NT_TRP!$A$2</definedName>
     <definedName name="ComTechs">#REF!</definedName>
@@ -215,7 +215,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1779" uniqueCount="352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1773" uniqueCount="352">
   <si>
     <t>BRT</t>
   </si>
@@ -1979,7 +1979,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="109">
+  <cellXfs count="108">
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -2158,9 +2158,6 @@
     <xf numFmtId="0" fontId="38" fillId="3" borderId="5" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="84">
     <cellStyle name="Calc" xfId="71" xr:uid="{41AB2454-0065-41FE-8ACF-05737930420F}"/>
@@ -2248,41 +2245,7 @@
     <cellStyle name="Percent 2" xfId="72" xr:uid="{035BF0CF-7219-469A-B7CE-DA974B61013B}"/>
     <cellStyle name="Währung_Excel2" xfId="58" xr:uid="{78A0101A-221E-43CC-8A5E-27AF7CEA13B7}"/>
   </cellStyles>
-  <dxfs count="8">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <fill>
         <patternFill>
@@ -7804,7 +7767,7 @@
   </sheetPr>
   <dimension ref="A1:O86"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
     <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="1">
@@ -7858,7 +7821,7 @@
         <v>77</v>
       </c>
       <c r="C2" s="30"/>
-      <c r="D2" s="108"/>
+      <c r="D2" s="101"/>
       <c r="E2" s="101"/>
       <c r="F2" s="87" t="s">
         <v>265</v>
@@ -11339,10 +11302,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F8:K83">
-    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="4">
+    <cfRule type="expression" dxfId="2" priority="4">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11356,10 +11319,10 @@
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
-  <dimension ref="A1:O86"/>
+  <dimension ref="A1:I84"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Q13" sqref="Q13"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
   </sheetViews>
@@ -11369,80 +11332,71 @@
     <col min="2" max="2" width="47.42578125" style="1" customWidth="1"/>
     <col min="3" max="4" width="19.42578125" style="1" customWidth="1"/>
     <col min="5" max="5" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14" style="26" customWidth="1"/>
-    <col min="7" max="15" width="10" style="1" customWidth="1"/>
-    <col min="16" max="16" width="9.140625" style="1" customWidth="1"/>
-    <col min="17" max="18" width="8.85546875" style="1"/>
-    <col min="19" max="19" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="8.85546875" style="1"/>
+    <col min="6" max="9" width="10" style="1" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" style="1" customWidth="1"/>
+    <col min="11" max="12" width="8.85546875" style="1"/>
+    <col min="13" max="13" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B1" s="25"/>
       <c r="C1" s="24"/>
       <c r="D1" s="24"/>
       <c r="E1" s="24"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
-      <c r="L1" s="23" t="s">
+      <c r="F1" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="M1" s="23" t="s">
+      <c r="G1" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="N1" s="23" t="s">
+      <c r="H1" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="O1" s="23" t="s">
+      <c r="I1" s="23" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="B2" s="21" t="s">
         <v>77</v>
       </c>
       <c r="C2" s="30"/>
-      <c r="D2" s="108"/>
-      <c r="E2" s="101"/>
-      <c r="F2" s="87" t="s">
+      <c r="D2" s="101"/>
+      <c r="E2" s="87" t="s">
         <v>265</v>
       </c>
-      <c r="G2" s="106" t="str">
+      <c r="F2" s="106" t="str">
         <f>CostProjections!M5</f>
         <v>NZE</v>
       </c>
-      <c r="H2" s="91" t="s">
+      <c r="G2" s="91" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="F3" s="88" t="s">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="E3" s="88" t="s">
         <v>266</v>
       </c>
-      <c r="G3" s="107" t="str">
+      <c r="F3" s="107" t="str">
         <f>CostProjections!M4</f>
         <v>NZE</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C4" s="97" t="s">
         <v>346</v>
       </c>
       <c r="D4" s="97"/>
-      <c r="E4" s="97"/>
-      <c r="F4" s="89" t="s">
+      <c r="E4" s="89" t="s">
         <v>267</v>
       </c>
-      <c r="G4" s="90">
+      <c r="F4" s="90">
         <f>CostProjections!M3</f>
         <v>2E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="98" t="s">
         <v>74</v>
       </c>
@@ -11455,38 +11409,20 @@
       <c r="E5" s="98" t="s">
         <v>344</v>
       </c>
-      <c r="F5" s="98" t="s">
-        <v>344</v>
-      </c>
-      <c r="G5" s="98" t="s">
-        <v>344</v>
-      </c>
-      <c r="H5" s="98" t="s">
-        <v>344</v>
-      </c>
-      <c r="I5" s="98" t="s">
-        <v>344</v>
-      </c>
-      <c r="J5" s="98" t="s">
-        <v>344</v>
-      </c>
-      <c r="K5" s="98" t="s">
-        <v>344</v>
-      </c>
-      <c r="L5" s="98">
+      <c r="F5" s="98">
         <v>2020</v>
       </c>
-      <c r="M5" s="98">
+      <c r="G5" s="98">
         <v>2030</v>
       </c>
-      <c r="N5" s="98">
+      <c r="H5" s="98">
         <v>2040</v>
       </c>
-      <c r="O5" s="98">
+      <c r="I5" s="98">
         <v>2050</v>
       </c>
     </row>
-    <row r="6" spans="1:15" s="17" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" s="17" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="17" t="s">
         <v>351</v>
       </c>
@@ -11504,34 +11440,16 @@
         <v>2020</v>
       </c>
       <c r="G6" s="19">
-        <v>2025</v>
+        <v>2030</v>
       </c>
       <c r="H6" s="19">
-        <v>2030</v>
+        <v>2040</v>
       </c>
       <c r="I6" s="19">
-        <v>2035</v>
-      </c>
-      <c r="J6" s="19">
-        <v>2040</v>
-      </c>
-      <c r="K6" s="19">
         <v>2050</v>
       </c>
-      <c r="L6" s="19">
-        <v>2020</v>
-      </c>
-      <c r="M6" s="19">
-        <v>2030</v>
-      </c>
-      <c r="N6" s="19">
-        <v>2040</v>
-      </c>
-      <c r="O6" s="19">
-        <v>2050</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
         <v>76</v>
       </c>
@@ -11545,14 +11463,8 @@
       <c r="G7" s="22"/>
       <c r="H7" s="22"/>
       <c r="I7" s="22"/>
-      <c r="J7" s="22"/>
-      <c r="K7" s="22"/>
-      <c r="L7" s="22"/>
-      <c r="M7" s="22"/>
-      <c r="N7" s="22"/>
-      <c r="O7" s="22"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>76</v>
       </c>
@@ -11568,30 +11480,24 @@
       <c r="E8" s="100" t="s">
         <v>13</v>
       </c>
-      <c r="F8" s="99"/>
-      <c r="G8" s="99"/>
-      <c r="H8" s="99"/>
-      <c r="I8" s="99"/>
-      <c r="J8" s="99"/>
-      <c r="K8" s="99"/>
-      <c r="L8" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C8,CostProjections!$L$11:$L$92,0),MATCH(L$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="F8" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C8,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>835.64408109927854</v>
       </c>
-      <c r="M8" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C8,CostProjections!$L$11:$L$92,0),MATCH(M$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="G8" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C8,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>852.50818368869375</v>
       </c>
-      <c r="N8" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C8,CostProjections!$L$11:$L$92,0),MATCH(N$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="H8" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C8,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>869.71262011470128</v>
       </c>
-      <c r="O8" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C8,CostProjections!$L$11:$L$92,0),MATCH(O$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="I8" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C8,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>887.26425864199052</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>76</v>
       </c>
@@ -11607,30 +11513,24 @@
       <c r="E9" s="100" t="s">
         <v>21</v>
       </c>
-      <c r="F9" s="99"/>
-      <c r="G9" s="99"/>
-      <c r="H9" s="99"/>
-      <c r="I9" s="99"/>
-      <c r="J9" s="99"/>
-      <c r="K9" s="99"/>
-      <c r="L9" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C9,CostProjections!$L$11:$L$92,0),MATCH(L$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="F9" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C9,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>438.90146207526243</v>
       </c>
-      <c r="M9" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C9,CostProjections!$L$11:$L$92,0),MATCH(M$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="G9" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C9,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>447.75891640359885</v>
       </c>
-      <c r="N9" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C9,CostProjections!$L$11:$L$92,0),MATCH(N$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="H9" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C9,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>456.79512269326983</v>
       </c>
-      <c r="O9" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C9,CostProjections!$L$11:$L$92,0),MATCH(O$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="I9" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C9,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>466.01368833105909</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B10" s="100" t="s">
         <v>80</v>
       </c>
@@ -11643,30 +11543,24 @@
       <c r="E10" s="100" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="99"/>
-      <c r="G10" s="99"/>
-      <c r="H10" s="99"/>
-      <c r="I10" s="99"/>
-      <c r="J10" s="99"/>
-      <c r="K10" s="99"/>
-      <c r="L10" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C10,CostProjections!$L$11:$L$92,0),MATCH(L$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="F10" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C10,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1115.3529863163551</v>
       </c>
-      <c r="M10" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C10,CostProjections!$L$11:$L$92,0),MATCH(M$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="G10" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C10,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>849.11877209576846</v>
       </c>
-      <c r="N10" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C10,CostProjections!$L$11:$L$92,0),MATCH(N$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="H10" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C10,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>851.93042365899805</v>
       </c>
-      <c r="O10" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C10,CostProjections!$L$11:$L$92,0),MATCH(O$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="I10" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C10,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>854.742075222229</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B11" s="100" t="s">
         <v>81</v>
       </c>
@@ -11679,30 +11573,24 @@
       <c r="E11" s="100" t="s">
         <v>21</v>
       </c>
-      <c r="F11" s="99"/>
-      <c r="G11" s="99"/>
-      <c r="H11" s="99"/>
-      <c r="I11" s="99"/>
-      <c r="J11" s="99"/>
-      <c r="K11" s="99"/>
-      <c r="L11" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C11,CostProjections!$L$11:$L$92,0),MATCH(L$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="F11" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C11,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>585.81167209404305</v>
       </c>
-      <c r="M11" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C11,CostProjections!$L$11:$L$92,0),MATCH(M$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="G11" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C11,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>445.97871148459467</v>
       </c>
-      <c r="N11" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C11,CostProjections!$L$11:$L$92,0),MATCH(N$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="H11" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C11,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>447.45546218487397</v>
       </c>
-      <c r="O11" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C11,CostProjections!$L$11:$L$92,0),MATCH(O$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="I11" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C11,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>448.93221288515406</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>76</v>
       </c>
@@ -11718,30 +11606,24 @@
       <c r="E12" s="100" t="s">
         <v>12</v>
       </c>
-      <c r="F12" s="99"/>
-      <c r="G12" s="99"/>
-      <c r="H12" s="99"/>
-      <c r="I12" s="99"/>
-      <c r="J12" s="99"/>
-      <c r="K12" s="99"/>
-      <c r="L12" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C12,CostProjections!$L$11:$L$92,0),MATCH(L$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="F12" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C12,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>919.2084892092065</v>
       </c>
-      <c r="M12" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C12,CostProjections!$L$11:$L$92,0),MATCH(M$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="G12" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C12,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>937.75900205756318</v>
       </c>
-      <c r="N12" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C12,CostProjections!$L$11:$L$92,0),MATCH(N$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="H12" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C12,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>956.68388212617151</v>
       </c>
-      <c r="O12" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C12,CostProjections!$L$11:$L$92,0),MATCH(O$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="I12" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C12,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>975.99068450618972</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B13" s="100" t="s">
         <v>83</v>
       </c>
@@ -11754,30 +11636,24 @@
       <c r="E13" s="100" t="s">
         <v>10</v>
       </c>
-      <c r="F13" s="99"/>
-      <c r="G13" s="99"/>
-      <c r="H13" s="99"/>
-      <c r="I13" s="99"/>
-      <c r="J13" s="99"/>
-      <c r="K13" s="99"/>
-      <c r="L13" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C13,CostProjections!$L$11:$L$92,0),MATCH(L$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="F13" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C13,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>3873.0540520727282</v>
       </c>
-      <c r="M13" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C13,CostProjections!$L$11:$L$92,0),MATCH(M$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="G13" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C13,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>2065.5976014079038</v>
       </c>
-      <c r="N13" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C13,CostProjections!$L$11:$L$92,0),MATCH(N$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="H13" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C13,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1939.8080038862586</v>
       </c>
-      <c r="O13" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C13,CostProjections!$L$11:$L$92,0),MATCH(O$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="I13" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C13,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1814.0184063646227</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>76</v>
       </c>
@@ -11793,30 +11669,24 @@
       <c r="E14" s="100" t="s">
         <v>11</v>
       </c>
-      <c r="F14" s="99"/>
-      <c r="G14" s="99"/>
-      <c r="H14" s="99"/>
-      <c r="I14" s="99"/>
-      <c r="J14" s="99"/>
-      <c r="K14" s="99"/>
-      <c r="L14" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C14,CostProjections!$L$11:$L$92,0),MATCH(L$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="F14" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C14,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>438.90146207526243</v>
       </c>
-      <c r="M14" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C14,CostProjections!$L$11:$L$92,0),MATCH(M$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="G14" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C14,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>447.75891640359885</v>
       </c>
-      <c r="N14" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C14,CostProjections!$L$11:$L$92,0),MATCH(N$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="H14" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C14,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>456.79512269326983</v>
       </c>
-      <c r="O14" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C14,CostProjections!$L$11:$L$92,0),MATCH(O$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="I14" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C14,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>466.01368833105909</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B15" s="100" t="s">
         <v>85</v>
       </c>
@@ -11829,30 +11699,24 @@
       <c r="E15" s="100" t="s">
         <v>9</v>
       </c>
-      <c r="F15" s="99"/>
-      <c r="G15" s="99"/>
-      <c r="H15" s="99"/>
-      <c r="I15" s="99"/>
-      <c r="J15" s="99"/>
-      <c r="K15" s="99"/>
-      <c r="L15" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C15,CostProjections!$L$11:$L$92,0),MATCH(L$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="F15" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C15,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1516.7538557832556</v>
       </c>
-      <c r="M15" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C15,CostProjections!$L$11:$L$92,0),MATCH(M$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="G15" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C15,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>808.92316097561422</v>
       </c>
-      <c r="N15" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C15,CostProjections!$L$11:$L$92,0),MATCH(N$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="H15" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C15,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>759.66181463414648</v>
       </c>
-      <c r="O15" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C15,CostProjections!$L$11:$L$92,0),MATCH(O$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="I15" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C15,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>710.40046829268272</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>76</v>
       </c>
@@ -11868,30 +11732,24 @@
       <c r="E16" s="100" t="s">
         <v>13</v>
       </c>
-      <c r="F16" s="99"/>
-      <c r="G16" s="99"/>
-      <c r="H16" s="99"/>
-      <c r="I16" s="99"/>
-      <c r="J16" s="99"/>
-      <c r="K16" s="99"/>
-      <c r="L16" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C16,CostProjections!$L$11:$L$92,0),MATCH(L$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="F16" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C16,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>656.10237784381934</v>
       </c>
-      <c r="M16" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C16,CostProjections!$L$11:$L$92,0),MATCH(M$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="G16" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C16,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>669.34315589679386</v>
       </c>
-      <c r="N16" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C16,CostProjections!$L$11:$L$92,0),MATCH(N$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="H16" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C16,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>682.85114560662009</v>
       </c>
-      <c r="O16" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C16,CostProjections!$L$11:$L$92,0),MATCH(O$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="I16" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C16,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>696.63173956195692</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>76</v>
       </c>
@@ -11907,30 +11765,24 @@
       <c r="E17" s="100" t="s">
         <v>21</v>
       </c>
-      <c r="F17" s="99"/>
-      <c r="G17" s="99"/>
-      <c r="H17" s="99"/>
-      <c r="I17" s="99"/>
-      <c r="J17" s="99"/>
-      <c r="K17" s="99"/>
-      <c r="L17" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C17,CostProjections!$L$11:$L$92,0),MATCH(L$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="F17" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C17,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>262.38470575580084</v>
       </c>
-      <c r="M17" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C17,CostProjections!$L$11:$L$92,0),MATCH(M$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="G17" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C17,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>267.67988189100242</v>
       </c>
-      <c r="N17" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C17,CostProjections!$L$11:$L$92,0),MATCH(N$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="H17" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C17,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>273.08191978181594</v>
       </c>
-      <c r="O17" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C17,CostProjections!$L$11:$L$92,0),MATCH(O$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="I17" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C17,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>278.59297600141696</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B18" s="100" t="s">
         <v>88</v>
       </c>
@@ -11943,30 +11795,24 @@
       <c r="E18" s="100" t="s">
         <v>13</v>
       </c>
-      <c r="F18" s="99"/>
-      <c r="G18" s="99"/>
-      <c r="H18" s="99"/>
-      <c r="I18" s="99"/>
-      <c r="J18" s="99"/>
-      <c r="K18" s="99"/>
-      <c r="L18" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C18,CostProjections!$L$11:$L$92,0),MATCH(L$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="F18" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C18,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1413.7180946041472</v>
       </c>
-      <c r="M18" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C18,CostProjections!$L$11:$L$92,0),MATCH(M$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="G18" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C18,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1076.264274455765</v>
       </c>
-      <c r="N18" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C18,CostProjections!$L$11:$L$92,0),MATCH(N$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="H18" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C18,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1079.8280634440273</v>
       </c>
-      <c r="O18" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C18,CostProjections!$L$11:$L$92,0),MATCH(O$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="I18" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C18,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1083.3918524322912</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B19" s="100" t="s">
         <v>89</v>
       </c>
@@ -11979,30 +11825,24 @@
       <c r="E19" s="100" t="s">
         <v>21</v>
       </c>
-      <c r="F19" s="99"/>
-      <c r="G19" s="99"/>
-      <c r="H19" s="99"/>
-      <c r="I19" s="99"/>
-      <c r="J19" s="99"/>
-      <c r="K19" s="99"/>
-      <c r="L19" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C19,CostProjections!$L$11:$L$92,0),MATCH(L$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="F19" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C19,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>565.36604469167128</v>
       </c>
-      <c r="M19" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C19,CostProjections!$L$11:$L$92,0),MATCH(M$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="G19" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C19,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>430.41344537815206</v>
       </c>
-      <c r="N19" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C19,CostProjections!$L$11:$L$92,0),MATCH(N$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="H19" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C19,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>431.83865546218487</v>
       </c>
-      <c r="O19" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C19,CostProjections!$L$11:$L$92,0),MATCH(O$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="I19" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C19,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>433.26386554621848</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B20" s="100" t="s">
         <v>90</v>
       </c>
@@ -12015,30 +11855,24 @@
       <c r="E20" s="100" t="s">
         <v>9</v>
       </c>
-      <c r="F20" s="99"/>
-      <c r="G20" s="99"/>
-      <c r="H20" s="99"/>
-      <c r="I20" s="99"/>
-      <c r="J20" s="99"/>
-      <c r="K20" s="99"/>
-      <c r="L20" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C20,CostProjections!$L$11:$L$92,0),MATCH(L$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="F20" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C20,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>996.58245713780525</v>
       </c>
-      <c r="M20" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C20,CostProjections!$L$11:$L$92,0),MATCH(M$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="G20" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C20,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>531.50260889526839</v>
       </c>
-      <c r="N20" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C20,CostProjections!$L$11:$L$92,0),MATCH(N$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="H20" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C20,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>499.13546284074624</v>
       </c>
-      <c r="O20" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C20,CostProjections!$L$11:$L$92,0),MATCH(O$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="I20" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C20,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>466.76831678622648</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>76</v>
       </c>
@@ -12054,30 +11888,24 @@
       <c r="E21" s="100" t="s">
         <v>12</v>
       </c>
-      <c r="F21" s="99"/>
-      <c r="G21" s="99"/>
-      <c r="H21" s="99"/>
-      <c r="I21" s="99"/>
-      <c r="J21" s="99"/>
-      <c r="K21" s="99"/>
-      <c r="L21" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C21,CostProjections!$L$11:$L$92,0),MATCH(L$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="F21" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C21,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>721.71261562820132</v>
       </c>
-      <c r="M21" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C21,CostProjections!$L$11:$L$92,0),MATCH(M$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="G21" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C21,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>736.27747148647325</v>
       </c>
-      <c r="N21" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C21,CostProjections!$L$11:$L$92,0),MATCH(N$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="H21" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C21,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>751.13626016728222</v>
       </c>
-      <c r="O21" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C21,CostProjections!$L$11:$L$92,0),MATCH(O$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="I21" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C21,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>766.29491351815273</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B22" s="100" t="s">
         <v>92</v>
       </c>
@@ -12090,30 +11918,24 @@
       <c r="E22" s="100" t="s">
         <v>10</v>
       </c>
-      <c r="F22" s="99"/>
-      <c r="G22" s="99"/>
-      <c r="H22" s="99"/>
-      <c r="I22" s="99"/>
-      <c r="J22" s="99"/>
-      <c r="K22" s="99"/>
-      <c r="L22" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C22,CostProjections!$L$11:$L$92,0),MATCH(L$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="F22" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C22,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>2544.7884698792823</v>
       </c>
-      <c r="M22" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C22,CostProjections!$L$11:$L$92,0),MATCH(M$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="G22" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C22,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1357.2000000000075</v>
       </c>
-      <c r="N22" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C22,CostProjections!$L$11:$L$92,0),MATCH(N$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="H22" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C22,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1274.5500000000002</v>
       </c>
-      <c r="O22" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C22,CostProjections!$L$11:$L$92,0),MATCH(O$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="I22" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C22,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1191.8999999999996</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>76</v>
       </c>
@@ -12129,30 +11951,24 @@
       <c r="E23" s="100" t="s">
         <v>11</v>
       </c>
-      <c r="F23" s="99"/>
-      <c r="G23" s="99"/>
-      <c r="H23" s="99"/>
-      <c r="I23" s="99"/>
-      <c r="J23" s="99"/>
-      <c r="K23" s="99"/>
-      <c r="L23" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C23,CostProjections!$L$11:$L$92,0),MATCH(L$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="F23" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C23,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>262.38470575580084</v>
       </c>
-      <c r="M23" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C23,CostProjections!$L$11:$L$92,0),MATCH(M$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="G23" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C23,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>267.67988189100242</v>
       </c>
-      <c r="N23" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C23,CostProjections!$L$11:$L$92,0),MATCH(N$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="H23" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C23,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>273.08191978181594</v>
       </c>
-      <c r="O23" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C23,CostProjections!$L$11:$L$92,0),MATCH(O$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="I23" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C23,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>278.59297600141696</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>76</v>
       </c>
@@ -12168,30 +11984,24 @@
       <c r="E24" s="100" t="s">
         <v>21</v>
       </c>
-      <c r="F24" s="99"/>
-      <c r="G24" s="99"/>
-      <c r="H24" s="99"/>
-      <c r="I24" s="99"/>
-      <c r="J24" s="99"/>
-      <c r="K24" s="99"/>
-      <c r="L24" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C24,CostProjections!$L$11:$L$92,0),MATCH(L$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="F24" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C24,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>140.61345431714946</v>
       </c>
-      <c r="M24" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C24,CostProjections!$L$11:$L$92,0),MATCH(M$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="G24" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C24,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>143.45116928778262</v>
       </c>
-      <c r="N24" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C24,CostProjections!$L$11:$L$92,0),MATCH(N$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="H24" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C24,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>146.34615208028723</v>
       </c>
-      <c r="O24" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C24,CostProjections!$L$11:$L$92,0),MATCH(O$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="I24" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C24,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>149.29955841447855</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B25" s="100" t="s">
         <v>95</v>
       </c>
@@ -12204,30 +12014,24 @@
       <c r="E25" s="100" t="s">
         <v>9</v>
       </c>
-      <c r="F25" s="99"/>
-      <c r="G25" s="99"/>
-      <c r="H25" s="99"/>
-      <c r="I25" s="99"/>
-      <c r="J25" s="99"/>
-      <c r="K25" s="99"/>
-      <c r="L25" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C25,CostProjections!$L$11:$L$92,0),MATCH(L$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="F25" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C25,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>201.43776538895028</v>
       </c>
-      <c r="M25" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C25,CostProjections!$L$11:$L$92,0),MATCH(M$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="G25" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C25,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>107.43185078909673</v>
       </c>
-      <c r="N25" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C25,CostProjections!$L$11:$L$92,0),MATCH(N$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="H25" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C25,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>100.88952654232429</v>
       </c>
-      <c r="O25" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C25,CostProjections!$L$11:$L$92,0),MATCH(O$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="I25" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C25,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>94.347202295552336</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>76</v>
       </c>
@@ -12243,30 +12047,24 @@
       <c r="E26" s="100" t="s">
         <v>13</v>
       </c>
-      <c r="F26" s="99"/>
-      <c r="G26" s="99"/>
-      <c r="H26" s="99"/>
-      <c r="I26" s="99"/>
-      <c r="J26" s="99"/>
-      <c r="K26" s="99"/>
-      <c r="L26" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C26,CostProjections!$L$11:$L$92,0),MATCH(L$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="F26" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C26,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1674.9173571001118</v>
       </c>
-      <c r="M26" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C26,CostProjections!$L$11:$L$92,0),MATCH(M$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="G26" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C26,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1708.7188029283056</v>
       </c>
-      <c r="N26" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C26,CostProjections!$L$11:$L$92,0),MATCH(N$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="H26" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C26,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1743.2023944965467</v>
       </c>
-      <c r="O26" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C26,CostProjections!$L$11:$L$92,0),MATCH(O$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="I26" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C26,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1778.3818981630261</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>76</v>
       </c>
@@ -12282,30 +12080,24 @@
       <c r="E27" s="100" t="s">
         <v>12</v>
       </c>
-      <c r="F27" s="99"/>
-      <c r="G27" s="99"/>
-      <c r="H27" s="99"/>
-      <c r="I27" s="99"/>
-      <c r="J27" s="99"/>
-      <c r="K27" s="99"/>
-      <c r="L27" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C27,CostProjections!$L$11:$L$92,0),MATCH(L$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="F27" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C27,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1775.901197692195</v>
       </c>
-      <c r="M27" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C27,CostProjections!$L$11:$L$92,0),MATCH(M$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="G27" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C27,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1811.7405947081456</v>
       </c>
-      <c r="N27" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C27,CostProjections!$L$11:$L$92,0),MATCH(N$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="H27" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C27,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1848.303265282409</v>
       </c>
-      <c r="O27" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C27,CostProjections!$L$11:$L$92,0),MATCH(O$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="I27" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C27,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1885.603805772171</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B28" s="100" t="s">
         <v>98</v>
       </c>
@@ -12318,30 +12110,24 @@
       <c r="E28" s="100" t="s">
         <v>10</v>
       </c>
-      <c r="F28" s="99"/>
-      <c r="G28" s="99"/>
-      <c r="H28" s="99"/>
-      <c r="I28" s="99"/>
-      <c r="J28" s="99"/>
-      <c r="K28" s="99"/>
-      <c r="L28" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C28,CostProjections!$L$11:$L$92,0),MATCH(L$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="F28" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C28,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>3448.5361583131421</v>
       </c>
-      <c r="M28" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C28,CostProjections!$L$11:$L$92,0),MATCH(M$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="G28" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C28,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1839.1914807302808</v>
       </c>
-      <c r="N28" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C28,CostProjections!$L$11:$L$92,0),MATCH(N$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="H28" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C28,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1727.1894354293891</v>
       </c>
-      <c r="O28" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C28,CostProjections!$L$11:$L$92,0),MATCH(O$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="I28" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C28,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1615.1873901285062</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>76</v>
       </c>
@@ -12357,30 +12143,24 @@
       <c r="E29" s="100" t="s">
         <v>11</v>
       </c>
-      <c r="F29" s="99"/>
-      <c r="G29" s="99"/>
-      <c r="H29" s="99"/>
-      <c r="I29" s="99"/>
-      <c r="J29" s="99"/>
-      <c r="K29" s="99"/>
-      <c r="L29" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C29,CostProjections!$L$11:$L$92,0),MATCH(L$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="F29" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C29,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1674.9173571001118</v>
       </c>
-      <c r="M29" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C29,CostProjections!$L$11:$L$92,0),MATCH(M$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="G29" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C29,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1708.7188029283056</v>
       </c>
-      <c r="N29" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C29,CostProjections!$L$11:$L$92,0),MATCH(N$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="H29" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C29,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1743.2023944965467</v>
       </c>
-      <c r="O29" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C29,CostProjections!$L$11:$L$92,0),MATCH(O$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="I29" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C29,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1778.3818981630261</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B30" s="100" t="s">
         <v>100</v>
       </c>
@@ -12393,30 +12173,24 @@
       <c r="E30" s="100" t="s">
         <v>9</v>
       </c>
-      <c r="F30" s="99"/>
-      <c r="G30" s="99"/>
-      <c r="H30" s="99"/>
-      <c r="I30" s="99"/>
-      <c r="J30" s="99"/>
-      <c r="K30" s="99"/>
-      <c r="L30" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C30,CostProjections!$L$11:$L$92,0),MATCH(L$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="F30" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C30,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>2885.1124291966107</v>
       </c>
-      <c r="M30" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C30,CostProjections!$L$11:$L$92,0),MATCH(M$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="G30" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C30,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1538.7033677857753</v>
       </c>
-      <c r="N30" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C30,CostProjections!$L$11:$L$92,0),MATCH(N$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="H30" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C30,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1445.0002780808647</v>
       </c>
-      <c r="O30" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C30,CostProjections!$L$11:$L$92,0),MATCH(O$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="I30" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C30,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1351.2971883759612</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>76</v>
       </c>
@@ -12432,30 +12206,24 @@
       <c r="E31" s="100" t="s">
         <v>13</v>
       </c>
-      <c r="F31" s="99"/>
-      <c r="G31" s="99"/>
-      <c r="H31" s="99"/>
-      <c r="I31" s="99"/>
-      <c r="J31" s="99"/>
-      <c r="K31" s="99"/>
-      <c r="L31" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C31,CostProjections!$L$11:$L$92,0),MATCH(L$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="F31" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C31,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>835.64408109927854</v>
       </c>
-      <c r="M31" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C31,CostProjections!$L$11:$L$92,0),MATCH(M$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="G31" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C31,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>852.50818368869375</v>
       </c>
-      <c r="N31" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C31,CostProjections!$L$11:$L$92,0),MATCH(N$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="H31" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C31,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>869.71262011470128</v>
       </c>
-      <c r="O31" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C31,CostProjections!$L$11:$L$92,0),MATCH(O$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="I31" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C31,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>887.26425864199052</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>76</v>
       </c>
@@ -12471,30 +12239,24 @@
       <c r="E32" s="100" t="s">
         <v>21</v>
       </c>
-      <c r="F32" s="99"/>
-      <c r="G32" s="99"/>
-      <c r="H32" s="99"/>
-      <c r="I32" s="99"/>
-      <c r="J32" s="99"/>
-      <c r="K32" s="99"/>
-      <c r="L32" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C32,CostProjections!$L$11:$L$92,0),MATCH(L$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="F32" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C32,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>438.90146207526243</v>
       </c>
-      <c r="M32" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C32,CostProjections!$L$11:$L$92,0),MATCH(M$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="G32" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C32,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>447.75891640359885</v>
       </c>
-      <c r="N32" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C32,CostProjections!$L$11:$L$92,0),MATCH(N$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="H32" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C32,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>456.79512269326983</v>
       </c>
-      <c r="O32" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C32,CostProjections!$L$11:$L$92,0),MATCH(O$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="I32" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C32,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>466.01368833105909</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>76</v>
       </c>
@@ -12510,30 +12272,24 @@
       <c r="E33" s="100" t="s">
         <v>12</v>
       </c>
-      <c r="F33" s="99"/>
-      <c r="G33" s="99"/>
-      <c r="H33" s="99"/>
-      <c r="I33" s="99"/>
-      <c r="J33" s="99"/>
-      <c r="K33" s="99"/>
-      <c r="L33" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C33,CostProjections!$L$11:$L$92,0),MATCH(L$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="F33" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C33,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>919.2084892092065</v>
       </c>
-      <c r="M33" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C33,CostProjections!$L$11:$L$92,0),MATCH(M$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="G33" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C33,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>937.75900205756318</v>
       </c>
-      <c r="N33" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C33,CostProjections!$L$11:$L$92,0),MATCH(N$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="H33" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C33,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>956.68388212617151</v>
       </c>
-      <c r="O33" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C33,CostProjections!$L$11:$L$92,0),MATCH(O$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="I33" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C33,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>975.99068450618972</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B34" s="100" t="s">
         <v>104</v>
       </c>
@@ -12546,30 +12302,24 @@
       <c r="E34" s="100" t="s">
         <v>10</v>
       </c>
-      <c r="F34" s="99"/>
-      <c r="G34" s="99"/>
-      <c r="H34" s="99"/>
-      <c r="I34" s="99"/>
-      <c r="J34" s="99"/>
-      <c r="K34" s="99"/>
-      <c r="L34" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C34,CostProjections!$L$11:$L$92,0),MATCH(L$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="F34" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C34,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>3873.0540520727282</v>
       </c>
-      <c r="M34" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C34,CostProjections!$L$11:$L$92,0),MATCH(M$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="G34" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C34,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>2065.5976014079038</v>
       </c>
-      <c r="N34" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C34,CostProjections!$L$11:$L$92,0),MATCH(N$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="H34" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C34,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1939.8080038862586</v>
       </c>
-      <c r="O34" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C34,CostProjections!$L$11:$L$92,0),MATCH(O$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="I34" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C34,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1814.0184063646227</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>76</v>
       </c>
@@ -12585,30 +12335,24 @@
       <c r="E35" s="100" t="s">
         <v>11</v>
       </c>
-      <c r="F35" s="99"/>
-      <c r="G35" s="99"/>
-      <c r="H35" s="99"/>
-      <c r="I35" s="99"/>
-      <c r="J35" s="99"/>
-      <c r="K35" s="99"/>
-      <c r="L35" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C35,CostProjections!$L$11:$L$92,0),MATCH(L$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="F35" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C35,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>438.90146207526243</v>
       </c>
-      <c r="M35" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C35,CostProjections!$L$11:$L$92,0),MATCH(M$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="G35" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C35,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>447.75891640359885</v>
       </c>
-      <c r="N35" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C35,CostProjections!$L$11:$L$92,0),MATCH(N$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="H35" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C35,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>456.79512269326983</v>
       </c>
-      <c r="O35" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C35,CostProjections!$L$11:$L$92,0),MATCH(O$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="I35" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C35,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>466.01368833105909</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B36" s="100" t="s">
         <v>106</v>
       </c>
@@ -12621,30 +12365,24 @@
       <c r="E36" s="100" t="s">
         <v>9</v>
       </c>
-      <c r="F36" s="99"/>
-      <c r="G36" s="99"/>
-      <c r="H36" s="99"/>
-      <c r="I36" s="99"/>
-      <c r="J36" s="99"/>
-      <c r="K36" s="99"/>
-      <c r="L36" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C36,CostProjections!$L$11:$L$92,0),MATCH(L$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="F36" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C36,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1516.7538557832556</v>
       </c>
-      <c r="M36" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C36,CostProjections!$L$11:$L$92,0),MATCH(M$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="G36" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C36,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>808.92316097561422</v>
       </c>
-      <c r="N36" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C36,CostProjections!$L$11:$L$92,0),MATCH(N$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="H36" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C36,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>759.66181463414648</v>
       </c>
-      <c r="O36" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C36,CostProjections!$L$11:$L$92,0),MATCH(O$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="I36" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C36,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>710.40046829268272</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>76</v>
       </c>
@@ -12660,30 +12398,24 @@
       <c r="E37" s="100" t="s">
         <v>13</v>
       </c>
-      <c r="F37" s="99"/>
-      <c r="G37" s="99"/>
-      <c r="H37" s="99"/>
-      <c r="I37" s="99"/>
-      <c r="J37" s="99"/>
-      <c r="K37" s="99"/>
-      <c r="L37" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C37,CostProjections!$L$11:$L$92,0),MATCH(L$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="F37" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C37,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1674.9173571001118</v>
       </c>
-      <c r="M37" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C37,CostProjections!$L$11:$L$92,0),MATCH(M$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="G37" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C37,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1708.7188029283056</v>
       </c>
-      <c r="N37" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C37,CostProjections!$L$11:$L$92,0),MATCH(N$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="H37" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C37,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1743.2023944965467</v>
       </c>
-      <c r="O37" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C37,CostProjections!$L$11:$L$92,0),MATCH(O$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="I37" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C37,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1778.3818981630261</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>76</v>
       </c>
@@ -12699,30 +12431,24 @@
       <c r="E38" s="100" t="s">
         <v>12</v>
       </c>
-      <c r="F38" s="99"/>
-      <c r="G38" s="99"/>
-      <c r="H38" s="99"/>
-      <c r="I38" s="99"/>
-      <c r="J38" s="99"/>
-      <c r="K38" s="99"/>
-      <c r="L38" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C38,CostProjections!$L$11:$L$92,0),MATCH(L$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="F38" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C38,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1775.901197692195</v>
       </c>
-      <c r="M38" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C38,CostProjections!$L$11:$L$92,0),MATCH(M$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="G38" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C38,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1811.7405947081456</v>
       </c>
-      <c r="N38" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C38,CostProjections!$L$11:$L$92,0),MATCH(N$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="H38" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C38,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1848.303265282409</v>
       </c>
-      <c r="O38" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C38,CostProjections!$L$11:$L$92,0),MATCH(O$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="I38" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C38,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1885.603805772171</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B39" s="100" t="s">
         <v>109</v>
       </c>
@@ -12735,30 +12461,24 @@
       <c r="E39" s="100" t="s">
         <v>9</v>
       </c>
-      <c r="F39" s="99"/>
-      <c r="G39" s="99"/>
-      <c r="H39" s="99"/>
-      <c r="I39" s="99"/>
-      <c r="J39" s="99"/>
-      <c r="K39" s="99"/>
-      <c r="L39" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C39,CostProjections!$L$11:$L$92,0),MATCH(L$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="F39" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C39,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>2885.1124291966107</v>
       </c>
-      <c r="M39" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C39,CostProjections!$L$11:$L$92,0),MATCH(M$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="G39" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C39,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1538.7033677857753</v>
       </c>
-      <c r="N39" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C39,CostProjections!$L$11:$L$92,0),MATCH(N$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="H39" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C39,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1445.0002780808647</v>
       </c>
-      <c r="O39" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C39,CostProjections!$L$11:$L$92,0),MATCH(O$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="I39" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C39,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1351.2971883759612</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B40" s="100" t="s">
         <v>110</v>
       </c>
@@ -12771,30 +12491,24 @@
       <c r="E40" s="100" t="s">
         <v>10</v>
       </c>
-      <c r="F40" s="99"/>
-      <c r="G40" s="99"/>
-      <c r="H40" s="99"/>
-      <c r="I40" s="99"/>
-      <c r="J40" s="99"/>
-      <c r="K40" s="99"/>
-      <c r="L40" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C40,CostProjections!$L$11:$L$92,0),MATCH(L$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="F40" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C40,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>3448.5361583131421</v>
       </c>
-      <c r="M40" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C40,CostProjections!$L$11:$L$92,0),MATCH(M$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="G40" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C40,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1839.1914807302808</v>
       </c>
-      <c r="N40" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C40,CostProjections!$L$11:$L$92,0),MATCH(N$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="H40" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C40,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1727.1894354293891</v>
       </c>
-      <c r="O40" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C40,CostProjections!$L$11:$L$92,0),MATCH(O$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="I40" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C40,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1615.1873901285062</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>76</v>
       </c>
@@ -12810,30 +12524,24 @@
       <c r="E41" s="100" t="s">
         <v>11</v>
       </c>
-      <c r="F41" s="99"/>
-      <c r="G41" s="99"/>
-      <c r="H41" s="99"/>
-      <c r="I41" s="99"/>
-      <c r="J41" s="99"/>
-      <c r="K41" s="99"/>
-      <c r="L41" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C41,CostProjections!$L$11:$L$92,0),MATCH(L$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="F41" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C41,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1674.9173571001118</v>
       </c>
-      <c r="M41" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C41,CostProjections!$L$11:$L$92,0),MATCH(M$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="G41" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C41,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1708.7188029283056</v>
       </c>
-      <c r="N41" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C41,CostProjections!$L$11:$L$92,0),MATCH(N$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="H41" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C41,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1743.2023944965467</v>
       </c>
-      <c r="O41" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C41,CostProjections!$L$11:$L$92,0),MATCH(O$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="I41" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C41,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1778.3818981630261</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>76</v>
       </c>
@@ -12849,30 +12557,24 @@
       <c r="E42" s="100" t="s">
         <v>13</v>
       </c>
-      <c r="F42" s="99"/>
-      <c r="G42" s="99"/>
-      <c r="H42" s="99"/>
-      <c r="I42" s="99"/>
-      <c r="J42" s="99"/>
-      <c r="K42" s="99"/>
-      <c r="L42" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C42,CostProjections!$L$11:$L$92,0),MATCH(L$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="F42" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C42,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>835.64408109927854</v>
       </c>
-      <c r="M42" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C42,CostProjections!$L$11:$L$92,0),MATCH(M$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="G42" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C42,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>852.50818368869375</v>
       </c>
-      <c r="N42" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C42,CostProjections!$L$11:$L$92,0),MATCH(N$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="H42" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C42,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>869.71262011470128</v>
       </c>
-      <c r="O42" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C42,CostProjections!$L$11:$L$92,0),MATCH(O$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="I42" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C42,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>887.26425864199052</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B43" s="100" t="s">
         <v>113</v>
       </c>
@@ -12885,30 +12587,24 @@
       <c r="E43" s="100" t="s">
         <v>13</v>
       </c>
-      <c r="F43" s="99"/>
-      <c r="G43" s="99"/>
-      <c r="H43" s="99"/>
-      <c r="I43" s="99"/>
-      <c r="J43" s="99"/>
-      <c r="K43" s="99"/>
-      <c r="L43" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C43,CostProjections!$L$11:$L$92,0),MATCH(L$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="F43" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C43,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1115.3529863163551</v>
       </c>
-      <c r="M43" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C43,CostProjections!$L$11:$L$92,0),MATCH(M$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="G43" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C43,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>849.11877209576846</v>
       </c>
-      <c r="N43" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C43,CostProjections!$L$11:$L$92,0),MATCH(N$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="H43" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C43,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>851.93042365899805</v>
       </c>
-      <c r="O43" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C43,CostProjections!$L$11:$L$92,0),MATCH(O$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="I43" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C43,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>854.742075222229</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>76</v>
       </c>
@@ -12924,30 +12620,24 @@
       <c r="E44" s="100" t="s">
         <v>21</v>
       </c>
-      <c r="F44" s="99"/>
-      <c r="G44" s="99"/>
-      <c r="H44" s="99"/>
-      <c r="I44" s="99"/>
-      <c r="J44" s="99"/>
-      <c r="K44" s="99"/>
-      <c r="L44" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C44,CostProjections!$L$11:$L$92,0),MATCH(L$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="F44" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C44,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>438.90146207526243</v>
       </c>
-      <c r="M44" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C44,CostProjections!$L$11:$L$92,0),MATCH(M$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="G44" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C44,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>447.75891640359885</v>
       </c>
-      <c r="N44" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C44,CostProjections!$L$11:$L$92,0),MATCH(N$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="H44" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C44,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>456.79512269326983</v>
       </c>
-      <c r="O44" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C44,CostProjections!$L$11:$L$92,0),MATCH(O$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="I44" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C44,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>466.01368833105909</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B45" s="100" t="s">
         <v>115</v>
       </c>
@@ -12960,30 +12650,24 @@
       <c r="E45" s="100" t="s">
         <v>21</v>
       </c>
-      <c r="F45" s="99"/>
-      <c r="G45" s="99"/>
-      <c r="H45" s="99"/>
-      <c r="I45" s="99"/>
-      <c r="J45" s="99"/>
-      <c r="K45" s="99"/>
-      <c r="L45" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C45,CostProjections!$L$11:$L$92,0),MATCH(L$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="F45" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C45,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>585.81167209404305</v>
       </c>
-      <c r="M45" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C45,CostProjections!$L$11:$L$92,0),MATCH(M$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="G45" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C45,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>445.97871148459467</v>
       </c>
-      <c r="N45" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C45,CostProjections!$L$11:$L$92,0),MATCH(N$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="H45" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C45,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>447.45546218487397</v>
       </c>
-      <c r="O45" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C45,CostProjections!$L$11:$L$92,0),MATCH(O$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="I45" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C45,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>448.93221288515406</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>76</v>
       </c>
@@ -12999,30 +12683,24 @@
       <c r="E46" s="100" t="s">
         <v>12</v>
       </c>
-      <c r="F46" s="99"/>
-      <c r="G46" s="99"/>
-      <c r="H46" s="99"/>
-      <c r="I46" s="99"/>
-      <c r="J46" s="99"/>
-      <c r="K46" s="99"/>
-      <c r="L46" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C46,CostProjections!$L$11:$L$92,0),MATCH(L$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="F46" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C46,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>919.2084892092065</v>
       </c>
-      <c r="M46" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C46,CostProjections!$L$11:$L$92,0),MATCH(M$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="G46" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C46,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>937.75900205756318</v>
       </c>
-      <c r="N46" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C46,CostProjections!$L$11:$L$92,0),MATCH(N$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="H46" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C46,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>956.68388212617151</v>
       </c>
-      <c r="O46" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C46,CostProjections!$L$11:$L$92,0),MATCH(O$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="I46" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C46,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>975.99068450618972</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B47" s="100" t="s">
         <v>117</v>
       </c>
@@ -13035,30 +12713,24 @@
       <c r="E47" s="100" t="s">
         <v>9</v>
       </c>
-      <c r="F47" s="99"/>
-      <c r="G47" s="99"/>
-      <c r="H47" s="99"/>
-      <c r="I47" s="99"/>
-      <c r="J47" s="99"/>
-      <c r="K47" s="99"/>
-      <c r="L47" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C47,CostProjections!$L$11:$L$92,0),MATCH(L$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="F47" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C47,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1516.7538557832556</v>
       </c>
-      <c r="M47" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C47,CostProjections!$L$11:$L$92,0),MATCH(M$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="G47" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C47,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>808.92316097561422</v>
       </c>
-      <c r="N47" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C47,CostProjections!$L$11:$L$92,0),MATCH(N$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="H47" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C47,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>759.66181463414648</v>
       </c>
-      <c r="O47" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C47,CostProjections!$L$11:$L$92,0),MATCH(O$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="I47" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C47,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>710.40046829268272</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>76</v>
       </c>
@@ -13074,30 +12746,24 @@
       <c r="E48" s="100" t="s">
         <v>13</v>
       </c>
-      <c r="F48" s="99"/>
-      <c r="G48" s="99"/>
-      <c r="H48" s="99"/>
-      <c r="I48" s="99"/>
-      <c r="J48" s="99"/>
-      <c r="K48" s="99"/>
-      <c r="L48" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C48,CostProjections!$L$11:$L$92,0),MATCH(L$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="F48" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C48,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>522.57584162425417</v>
       </c>
-      <c r="M48" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C48,CostProjections!$L$11:$L$92,0),MATCH(M$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="G48" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C48,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>533.12192554111539</v>
       </c>
-      <c r="N48" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C48,CostProjections!$L$11:$L$92,0),MATCH(N$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="H48" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C48,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>543.88083959117944</v>
       </c>
-      <c r="O48" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C48,CostProjections!$L$11:$L$92,0),MATCH(O$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="I48" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C48,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>554.85687889156804</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>76</v>
       </c>
@@ -13113,30 +12779,24 @@
       <c r="E49" s="100" t="s">
         <v>21</v>
       </c>
-      <c r="F49" s="99"/>
-      <c r="G49" s="99"/>
-      <c r="H49" s="99"/>
-      <c r="I49" s="99"/>
-      <c r="J49" s="99"/>
-      <c r="K49" s="99"/>
-      <c r="L49" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C49,CostProjections!$L$11:$L$92,0),MATCH(L$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="F49" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C49,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>411.73058994760896</v>
       </c>
-      <c r="M49" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C49,CostProjections!$L$11:$L$92,0),MATCH(M$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="G49" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C49,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>420.0397099008585</v>
       </c>
-      <c r="N49" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C49,CostProjections!$L$11:$L$92,0),MATCH(N$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="H49" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C49,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>428.51651589950546</v>
       </c>
-      <c r="O49" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C49,CostProjections!$L$11:$L$92,0),MATCH(O$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="I49" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C49,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>437.16439200948946</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>76</v>
       </c>
@@ -13152,30 +12812,24 @@
       <c r="E50" s="100" t="s">
         <v>13</v>
       </c>
-      <c r="F50" s="99"/>
-      <c r="G50" s="99"/>
-      <c r="H50" s="99"/>
-      <c r="I50" s="99"/>
-      <c r="J50" s="99"/>
-      <c r="K50" s="99"/>
-      <c r="L50" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C50,CostProjections!$L$11:$L$92,0),MATCH(L$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="F50" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C50,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>522.57584162425417</v>
       </c>
-      <c r="M50" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C50,CostProjections!$L$11:$L$92,0),MATCH(M$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="G50" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C50,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>533.12192554111539</v>
       </c>
-      <c r="N50" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C50,CostProjections!$L$11:$L$92,0),MATCH(N$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="H50" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C50,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>543.88083959117944</v>
       </c>
-      <c r="O50" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C50,CostProjections!$L$11:$L$92,0),MATCH(O$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="I50" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C50,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>554.85687889156804</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>76</v>
       </c>
@@ -13191,30 +12845,24 @@
       <c r="E51" s="100" t="s">
         <v>13</v>
       </c>
-      <c r="F51" s="99"/>
-      <c r="G51" s="99"/>
-      <c r="H51" s="99"/>
-      <c r="I51" s="99"/>
-      <c r="J51" s="99"/>
-      <c r="K51" s="99"/>
-      <c r="L51" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C51,CostProjections!$L$11:$L$92,0),MATCH(L$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="F51" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C51,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>522.57584162425417</v>
       </c>
-      <c r="M51" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C51,CostProjections!$L$11:$L$92,0),MATCH(M$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="G51" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C51,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>533.12192554111539</v>
       </c>
-      <c r="N51" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C51,CostProjections!$L$11:$L$92,0),MATCH(N$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="H51" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C51,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>543.88083959117944</v>
       </c>
-      <c r="O51" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C51,CostProjections!$L$11:$L$92,0),MATCH(O$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="I51" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C51,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>554.85687889156804</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>76</v>
       </c>
@@ -13230,30 +12878,24 @@
       <c r="E52" s="100" t="s">
         <v>13</v>
       </c>
-      <c r="F52" s="99"/>
-      <c r="G52" s="99"/>
-      <c r="H52" s="99"/>
-      <c r="I52" s="99"/>
-      <c r="J52" s="99"/>
-      <c r="K52" s="99"/>
-      <c r="L52" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C52,CostProjections!$L$11:$L$92,0),MATCH(L$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="F52" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C52,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>902.73536260054868</v>
       </c>
-      <c r="M52" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C52,CostProjections!$L$11:$L$92,0),MATCH(M$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="G52" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C52,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>920.95343188425818</v>
       </c>
-      <c r="N52" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C52,CostProjections!$L$11:$L$92,0),MATCH(N$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="H52" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C52,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>939.53915935681937</v>
       </c>
-      <c r="O52" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C52,CostProjections!$L$11:$L$92,0),MATCH(O$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="I52" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C52,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>958.49996471467352</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>76</v>
       </c>
@@ -13269,30 +12911,24 @@
       <c r="E53" s="100" t="s">
         <v>13</v>
       </c>
-      <c r="F53" s="99"/>
-      <c r="G53" s="99"/>
-      <c r="H53" s="99"/>
-      <c r="I53" s="99"/>
-      <c r="J53" s="99"/>
-      <c r="K53" s="99"/>
-      <c r="L53" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C53,CostProjections!$L$11:$L$92,0),MATCH(L$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="F53" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C53,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>858.22359532891846</v>
       </c>
-      <c r="M53" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C53,CostProjections!$L$11:$L$92,0),MATCH(M$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="G53" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C53,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>875.54337426787095</v>
       </c>
-      <c r="N53" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C53,CostProjections!$L$11:$L$92,0),MATCH(N$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="H53" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C53,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>893.21268303113357</v>
       </c>
-      <c r="O53" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C53,CostProjections!$L$11:$L$92,0),MATCH(O$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="I53" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C53,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>911.23857546728675</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>76</v>
       </c>
@@ -13308,30 +12944,24 @@
       <c r="E54" s="100" t="s">
         <v>13</v>
       </c>
-      <c r="F54" s="99"/>
-      <c r="G54" s="99"/>
-      <c r="H54" s="99"/>
-      <c r="I54" s="99"/>
-      <c r="J54" s="99"/>
-      <c r="K54" s="99"/>
-      <c r="L54" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C54,CostProjections!$L$11:$L$92,0),MATCH(L$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="F54" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C54,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>858.22359532891846</v>
       </c>
-      <c r="M54" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C54,CostProjections!$L$11:$L$92,0),MATCH(M$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="G54" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C54,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>875.54337426787095</v>
       </c>
-      <c r="N54" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C54,CostProjections!$L$11:$L$92,0),MATCH(N$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="H54" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C54,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>893.21268303113357</v>
       </c>
-      <c r="O54" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C54,CostProjections!$L$11:$L$92,0),MATCH(O$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="I54" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C54,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>911.23857546728675</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>76</v>
       </c>
@@ -13347,30 +12977,24 @@
       <c r="E55" s="100" t="s">
         <v>13</v>
       </c>
-      <c r="F55" s="99"/>
-      <c r="G55" s="99"/>
-      <c r="H55" s="99"/>
-      <c r="I55" s="99"/>
-      <c r="J55" s="99"/>
-      <c r="K55" s="99"/>
-      <c r="L55" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C55,CostProjections!$L$11:$L$92,0),MATCH(L$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="F55" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C55,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1128.5294733678718</v>
       </c>
-      <c r="M55" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C55,CostProjections!$L$11:$L$92,0),MATCH(M$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="G55" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C55,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1151.3042853297043</v>
       </c>
-      <c r="N55" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C55,CostProjections!$L$11:$L$92,0),MATCH(N$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="H55" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C55,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1174.5387149374535</v>
       </c>
-      <c r="O55" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C55,CostProjections!$L$11:$L$92,0),MATCH(O$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="I55" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C55,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1198.2420377179947</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>76</v>
       </c>
@@ -13386,30 +13010,24 @@
       <c r="E56" s="100" t="s">
         <v>13</v>
       </c>
-      <c r="F56" s="99"/>
-      <c r="G56" s="99"/>
-      <c r="H56" s="99"/>
-      <c r="I56" s="99"/>
-      <c r="J56" s="99"/>
-      <c r="K56" s="99"/>
-      <c r="L56" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C56,CostProjections!$L$11:$L$92,0),MATCH(L$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="F56" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C56,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1128.5294733678718</v>
       </c>
-      <c r="M56" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C56,CostProjections!$L$11:$L$92,0),MATCH(M$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="G56" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C56,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1151.3042853297043</v>
       </c>
-      <c r="N56" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C56,CostProjections!$L$11:$L$92,0),MATCH(N$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="H56" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C56,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1174.5387149374535</v>
       </c>
-      <c r="O56" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C56,CostProjections!$L$11:$L$92,0),MATCH(O$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="I56" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C56,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1198.2420377179947</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>76</v>
       </c>
@@ -13425,30 +13043,24 @@
       <c r="E57" s="100" t="s">
         <v>13</v>
       </c>
-      <c r="F57" s="99"/>
-      <c r="G57" s="99"/>
-      <c r="H57" s="99"/>
-      <c r="I57" s="99"/>
-      <c r="J57" s="99"/>
-      <c r="K57" s="99"/>
-      <c r="L57" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C57,CostProjections!$L$11:$L$92,0),MATCH(L$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="F57" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C57,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1128.5294733678718</v>
       </c>
-      <c r="M57" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C57,CostProjections!$L$11:$L$92,0),MATCH(M$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="G57" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C57,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1151.3042853297043</v>
       </c>
-      <c r="N57" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C57,CostProjections!$L$11:$L$92,0),MATCH(N$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="H57" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C57,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1174.5387149374535</v>
       </c>
-      <c r="O57" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C57,CostProjections!$L$11:$L$92,0),MATCH(O$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="I57" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C57,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1198.2420377179947</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>76</v>
       </c>
@@ -13464,30 +13076,24 @@
       <c r="E58" s="100" t="s">
         <v>12</v>
       </c>
-      <c r="F58" s="99"/>
-      <c r="G58" s="99"/>
-      <c r="H58" s="99"/>
-      <c r="I58" s="99"/>
-      <c r="J58" s="99"/>
-      <c r="K58" s="99"/>
-      <c r="L58" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C58,CostProjections!$L$11:$L$92,0),MATCH(L$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="F58" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C58,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>645.6084743842323</v>
       </c>
-      <c r="M58" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C58,CostProjections!$L$11:$L$92,0),MATCH(M$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="G58" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C58,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>658.63747535590073</v>
       </c>
-      <c r="N58" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C58,CostProjections!$L$11:$L$92,0),MATCH(N$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="H58" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C58,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>671.92941411890092</v>
       </c>
-      <c r="O58" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C58,CostProjections!$L$11:$L$92,0),MATCH(O$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="I58" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C58,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>685.48959701116814</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>76</v>
       </c>
@@ -13503,30 +13109,24 @@
       <c r="E59" s="100" t="s">
         <v>12</v>
       </c>
-      <c r="F59" s="99"/>
-      <c r="G59" s="99"/>
-      <c r="H59" s="99"/>
-      <c r="I59" s="99"/>
-      <c r="J59" s="99"/>
-      <c r="K59" s="99"/>
-      <c r="L59" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C59,CostProjections!$L$11:$L$92,0),MATCH(L$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="F59" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C59,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>645.6084743842323</v>
       </c>
-      <c r="M59" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C59,CostProjections!$L$11:$L$92,0),MATCH(M$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="G59" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C59,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>658.63747535590073</v>
       </c>
-      <c r="N59" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C59,CostProjections!$L$11:$L$92,0),MATCH(N$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="H59" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C59,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>671.92941411890092</v>
       </c>
-      <c r="O59" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C59,CostProjections!$L$11:$L$92,0),MATCH(O$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="I59" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C59,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>685.48959701116814</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>76</v>
       </c>
@@ -13542,30 +13142,24 @@
       <c r="E60" s="100" t="s">
         <v>12</v>
       </c>
-      <c r="F60" s="99"/>
-      <c r="G60" s="99"/>
-      <c r="H60" s="99"/>
-      <c r="I60" s="99"/>
-      <c r="J60" s="99"/>
-      <c r="K60" s="99"/>
-      <c r="L60" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C60,CostProjections!$L$11:$L$92,0),MATCH(L$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="F60" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C60,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>645.6084743842323</v>
       </c>
-      <c r="M60" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C60,CostProjections!$L$11:$L$92,0),MATCH(M$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="G60" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C60,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>658.63747535590073</v>
       </c>
-      <c r="N60" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C60,CostProjections!$L$11:$L$92,0),MATCH(N$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="H60" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C60,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>671.92941411890092</v>
       </c>
-      <c r="O60" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C60,CostProjections!$L$11:$L$92,0),MATCH(O$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="I60" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C60,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>685.48959701116814</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>76</v>
       </c>
@@ -13581,30 +13175,24 @@
       <c r="E61" s="100" t="s">
         <v>12</v>
       </c>
-      <c r="F61" s="99"/>
-      <c r="G61" s="99"/>
-      <c r="H61" s="99"/>
-      <c r="I61" s="99"/>
-      <c r="J61" s="99"/>
-      <c r="K61" s="99"/>
-      <c r="L61" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C61,CostProjections!$L$11:$L$92,0),MATCH(L$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="F61" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C61,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1086.2358398404897</v>
       </c>
-      <c r="M61" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C61,CostProjections!$L$11:$L$92,0),MATCH(M$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="G61" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C61,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1108.1571255334031</v>
       </c>
-      <c r="N61" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C61,CostProjections!$L$11:$L$92,0),MATCH(N$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="H61" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C61,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1130.5208038898666</v>
       </c>
-      <c r="O61" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C61,CostProjections!$L$11:$L$92,0),MATCH(O$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="I61" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C61,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1153.3358028200171</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>76</v>
       </c>
@@ -13620,30 +13208,24 @@
       <c r="E62" s="100" t="s">
         <v>12</v>
       </c>
-      <c r="F62" s="99"/>
-      <c r="G62" s="99"/>
-      <c r="H62" s="99"/>
-      <c r="I62" s="99"/>
-      <c r="J62" s="99"/>
-      <c r="K62" s="99"/>
-      <c r="L62" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C62,CostProjections!$L$11:$L$92,0),MATCH(L$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="F62" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C62,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>991.12866157757253</v>
       </c>
-      <c r="M62" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C62,CostProjections!$L$11:$L$92,0),MATCH(M$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="G62" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C62,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1011.130592789921</v>
       </c>
-      <c r="N62" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C62,CostProjections!$L$11:$L$92,0),MATCH(N$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="H62" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C62,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1031.5361822433565</v>
       </c>
-      <c r="O62" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C62,CostProjections!$L$11:$L$92,0),MATCH(O$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="I62" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C62,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1052.3535761500559</v>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>76</v>
       </c>
@@ -13659,30 +13241,24 @@
       <c r="E63" s="100" t="s">
         <v>12</v>
       </c>
-      <c r="F63" s="99"/>
-      <c r="G63" s="99"/>
-      <c r="H63" s="99"/>
-      <c r="I63" s="99"/>
-      <c r="J63" s="99"/>
-      <c r="K63" s="99"/>
-      <c r="L63" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C63,CostProjections!$L$11:$L$92,0),MATCH(L$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="F63" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C63,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>991.12866157757253</v>
       </c>
-      <c r="M63" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C63,CostProjections!$L$11:$L$92,0),MATCH(M$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="G63" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C63,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1011.130592789921</v>
       </c>
-      <c r="N63" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C63,CostProjections!$L$11:$L$92,0),MATCH(N$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="H63" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C63,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1031.5361822433565</v>
       </c>
-      <c r="O63" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C63,CostProjections!$L$11:$L$92,0),MATCH(O$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="I63" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C63,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1052.3535761500559</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>76</v>
       </c>
@@ -13698,30 +13274,24 @@
       <c r="E64" s="100" t="s">
         <v>12</v>
       </c>
-      <c r="F64" s="99"/>
-      <c r="G64" s="99"/>
-      <c r="H64" s="99"/>
-      <c r="I64" s="99"/>
-      <c r="J64" s="99"/>
-      <c r="K64" s="99"/>
-      <c r="L64" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C64,CostProjections!$L$11:$L$92,0),MATCH(L$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="F64" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C64,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1308.7827191732849</v>
       </c>
-      <c r="M64" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C64,CostProjections!$L$11:$L$92,0),MATCH(M$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="G64" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C64,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1335.1952152856936</v>
       </c>
-      <c r="N64" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C64,CostProjections!$L$11:$L$92,0),MATCH(N$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="H64" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C64,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1362.1407410146062</v>
       </c>
-      <c r="O64" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C64,CostProjections!$L$11:$L$92,0),MATCH(O$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="I64" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C64,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1389.6300534111874</v>
       </c>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>76</v>
       </c>
@@ -13737,30 +13307,24 @@
       <c r="E65" s="100" t="s">
         <v>12</v>
       </c>
-      <c r="F65" s="99"/>
-      <c r="G65" s="99"/>
-      <c r="H65" s="99"/>
-      <c r="I65" s="99"/>
-      <c r="J65" s="99"/>
-      <c r="K65" s="99"/>
-      <c r="L65" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C65,CostProjections!$L$11:$L$92,0),MATCH(L$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="F65" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C65,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1308.7827191732849</v>
       </c>
-      <c r="M65" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C65,CostProjections!$L$11:$L$92,0),MATCH(M$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="G65" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C65,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1335.1952152856936</v>
       </c>
-      <c r="N65" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C65,CostProjections!$L$11:$L$92,0),MATCH(N$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="H65" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C65,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1362.1407410146062</v>
       </c>
-      <c r="O65" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C65,CostProjections!$L$11:$L$92,0),MATCH(O$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="I65" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C65,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1389.6300534111874</v>
       </c>
     </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>76</v>
       </c>
@@ -13776,30 +13340,24 @@
       <c r="E66" s="100" t="s">
         <v>12</v>
       </c>
-      <c r="F66" s="99"/>
-      <c r="G66" s="99"/>
-      <c r="H66" s="99"/>
-      <c r="I66" s="99"/>
-      <c r="J66" s="99"/>
-      <c r="K66" s="99"/>
-      <c r="L66" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C66,CostProjections!$L$11:$L$92,0),MATCH(L$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="F66" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C66,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1308.7827191732849</v>
       </c>
-      <c r="M66" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C66,CostProjections!$L$11:$L$92,0),MATCH(M$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="G66" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C66,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1335.1952152856936</v>
       </c>
-      <c r="N66" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C66,CostProjections!$L$11:$L$92,0),MATCH(N$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="H66" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C66,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1362.1407410146062</v>
       </c>
-      <c r="O66" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C66,CostProjections!$L$11:$L$92,0),MATCH(O$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="I66" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C66,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1389.6300534111874</v>
       </c>
     </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B67" s="100" t="s">
         <v>137</v>
       </c>
@@ -13812,30 +13370,24 @@
       <c r="E67" s="100" t="s">
         <v>9</v>
       </c>
-      <c r="F67" s="99"/>
-      <c r="G67" s="99"/>
-      <c r="H67" s="99"/>
-      <c r="I67" s="99"/>
-      <c r="J67" s="99"/>
-      <c r="K67" s="99"/>
-      <c r="L67" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C67,CostProjections!$L$11:$L$92,0),MATCH(L$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="F67" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C67,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1161.917203295312</v>
       </c>
-      <c r="M67" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C67,CostProjections!$L$11:$L$92,0),MATCH(M$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="G67" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C67,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>619.67980717360467</v>
       </c>
-      <c r="N67" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C67,CostProjections!$L$11:$L$92,0),MATCH(N$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="H67" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C67,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>581.94289583931152</v>
       </c>
-      <c r="O67" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C67,CostProjections!$L$11:$L$92,0),MATCH(O$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="I67" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C67,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>544.20598450502132</v>
       </c>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B68" s="100" t="s">
         <v>138</v>
       </c>
@@ -13848,30 +13400,24 @@
       <c r="E68" s="100" t="s">
         <v>9</v>
       </c>
-      <c r="F68" s="99"/>
-      <c r="G68" s="99"/>
-      <c r="H68" s="99"/>
-      <c r="I68" s="99"/>
-      <c r="J68" s="99"/>
-      <c r="K68" s="99"/>
-      <c r="L68" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C68,CostProjections!$L$11:$L$92,0),MATCH(L$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="F68" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C68,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1161.917203295312</v>
       </c>
-      <c r="M68" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C68,CostProjections!$L$11:$L$92,0),MATCH(M$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="G68" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C68,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>619.67980717360467</v>
       </c>
-      <c r="N68" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C68,CostProjections!$L$11:$L$92,0),MATCH(N$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="H68" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C68,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>581.94289583931152</v>
       </c>
-      <c r="O68" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C68,CostProjections!$L$11:$L$92,0),MATCH(O$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="I68" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C68,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>544.20598450502132</v>
       </c>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B69" s="100" t="s">
         <v>139</v>
       </c>
@@ -13884,30 +13430,24 @@
       <c r="E69" s="100" t="s">
         <v>9</v>
       </c>
-      <c r="F69" s="99"/>
-      <c r="G69" s="99"/>
-      <c r="H69" s="99"/>
-      <c r="I69" s="99"/>
-      <c r="J69" s="99"/>
-      <c r="K69" s="99"/>
-      <c r="L69" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C69,CostProjections!$L$11:$L$92,0),MATCH(L$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="F69" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C69,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1161.917203295312</v>
       </c>
-      <c r="M69" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C69,CostProjections!$L$11:$L$92,0),MATCH(M$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="G69" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C69,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>619.67980717360467</v>
       </c>
-      <c r="N69" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C69,CostProjections!$L$11:$L$92,0),MATCH(N$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="H69" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C69,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>581.94289583931152</v>
       </c>
-      <c r="O69" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C69,CostProjections!$L$11:$L$92,0),MATCH(O$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="I69" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C69,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>544.20598450502132</v>
       </c>
     </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B70" s="100" t="s">
         <v>185</v>
       </c>
@@ -13920,30 +13460,24 @@
       <c r="E70" s="100" t="s">
         <v>9</v>
       </c>
-      <c r="F70" s="99"/>
-      <c r="G70" s="99"/>
-      <c r="H70" s="99"/>
-      <c r="I70" s="99"/>
-      <c r="J70" s="99"/>
-      <c r="K70" s="99"/>
-      <c r="L70" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C70,CostProjections!$L$11:$L$92,0),MATCH(L$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="F70" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C70,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>2007.179942663324</v>
       </c>
-      <c r="M70" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C70,CostProjections!$L$11:$L$92,0),MATCH(M$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="G70" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C70,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1070.4797866016361</v>
       </c>
-      <c r="N70" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C70,CostProjections!$L$11:$L$92,0),MATCH(N$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="H70" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C70,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1005.2903124175569</v>
       </c>
-      <c r="O70" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C70,CostProjections!$L$11:$L$92,0),MATCH(O$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="I70" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C70,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>940.10083823348259</v>
       </c>
     </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B71" s="100" t="s">
         <v>186</v>
       </c>
@@ -13956,30 +13490,24 @@
       <c r="E71" s="100" t="s">
         <v>9</v>
       </c>
-      <c r="F71" s="99"/>
-      <c r="G71" s="99"/>
-      <c r="H71" s="99"/>
-      <c r="I71" s="99"/>
-      <c r="J71" s="99"/>
-      <c r="K71" s="99"/>
-      <c r="L71" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C71,CostProjections!$L$11:$L$92,0),MATCH(L$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="F71" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C71,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1908.21059884285</v>
       </c>
-      <c r="M71" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C71,CostProjections!$L$11:$L$92,0),MATCH(M$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="G71" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C71,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1017.6969345009586</v>
       </c>
-      <c r="N71" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C71,CostProjections!$L$11:$L$92,0),MATCH(N$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="H71" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C71,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>955.72180066916428</v>
       </c>
-      <c r="O71" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C71,CostProjections!$L$11:$L$92,0),MATCH(O$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="I71" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C71,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>893.74666683737496</v>
       </c>
     </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B72" s="100" t="s">
         <v>187</v>
       </c>
@@ -13992,30 +13520,24 @@
       <c r="E72" s="100" t="s">
         <v>9</v>
       </c>
-      <c r="F72" s="99"/>
-      <c r="G72" s="99"/>
-      <c r="H72" s="99"/>
-      <c r="I72" s="99"/>
-      <c r="J72" s="99"/>
-      <c r="K72" s="99"/>
-      <c r="L72" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C72,CostProjections!$L$11:$L$92,0),MATCH(L$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="F72" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C72,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1908.21059884285</v>
       </c>
-      <c r="M72" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C72,CostProjections!$L$11:$L$92,0),MATCH(M$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="G72" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C72,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1017.6969345009586</v>
       </c>
-      <c r="N72" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C72,CostProjections!$L$11:$L$92,0),MATCH(N$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="H72" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C72,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>955.72180066916428</v>
       </c>
-      <c r="O72" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C72,CostProjections!$L$11:$L$92,0),MATCH(O$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="I72" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C72,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>893.74666683737496</v>
       </c>
     </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B73" s="100" t="s">
         <v>188</v>
       </c>
@@ -14028,30 +13550,24 @@
       <c r="E73" s="100" t="s">
         <v>9</v>
       </c>
-      <c r="F73" s="99"/>
-      <c r="G73" s="99"/>
-      <c r="H73" s="99"/>
-      <c r="I73" s="99"/>
-      <c r="J73" s="99"/>
-      <c r="K73" s="99"/>
-      <c r="L73" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C73,CostProjections!$L$11:$L$92,0),MATCH(L$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="F73" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C73,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>2509.2201075662383</v>
       </c>
-      <c r="M73" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C73,CostProjections!$L$11:$L$92,0),MATCH(M$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="G73" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C73,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1338.2304935350739</v>
       </c>
-      <c r="N73" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C73,CostProjections!$L$11:$L$92,0),MATCH(N$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="H73" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C73,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1256.7356878390212</v>
       </c>
-      <c r="O73" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C73,CostProjections!$L$11:$L$92,0),MATCH(O$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="I73" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C73,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1175.2408821429744</v>
       </c>
     </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B74" s="100" t="s">
         <v>189</v>
       </c>
@@ -14064,30 +13580,24 @@
       <c r="E74" s="100" t="s">
         <v>9</v>
       </c>
-      <c r="F74" s="99"/>
-      <c r="G74" s="99"/>
-      <c r="H74" s="99"/>
-      <c r="I74" s="99"/>
-      <c r="J74" s="99"/>
-      <c r="K74" s="99"/>
-      <c r="L74" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C74,CostProjections!$L$11:$L$92,0),MATCH(L$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="F74" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C74,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>2509.2201075662383</v>
       </c>
-      <c r="M74" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C74,CostProjections!$L$11:$L$92,0),MATCH(M$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="G74" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C74,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1338.2304935350739</v>
       </c>
-      <c r="N74" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C74,CostProjections!$L$11:$L$92,0),MATCH(N$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="H74" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C74,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1256.7356878390212</v>
       </c>
-      <c r="O74" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C74,CostProjections!$L$11:$L$92,0),MATCH(O$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="I74" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C74,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1175.2408821429744</v>
       </c>
     </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B75" s="100" t="s">
         <v>190</v>
       </c>
@@ -14100,30 +13610,24 @@
       <c r="E75" s="100" t="s">
         <v>9</v>
       </c>
-      <c r="F75" s="99"/>
-      <c r="G75" s="99"/>
-      <c r="H75" s="99"/>
-      <c r="I75" s="99"/>
-      <c r="J75" s="99"/>
-      <c r="K75" s="99"/>
-      <c r="L75" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C75,CostProjections!$L$11:$L$92,0),MATCH(L$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="F75" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C75,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>2509.2201075662383</v>
       </c>
-      <c r="M75" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C75,CostProjections!$L$11:$L$92,0),MATCH(M$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="G75" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C75,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1338.2304935350739</v>
       </c>
-      <c r="N75" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C75,CostProjections!$L$11:$L$92,0),MATCH(N$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="H75" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C75,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1256.7356878390212</v>
       </c>
-      <c r="O75" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C75,CostProjections!$L$11:$L$92,0),MATCH(O$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="I75" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C75,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1175.2408821429744</v>
       </c>
     </row>
-    <row r="76" spans="1:15" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B76" s="100" t="s">
         <v>140</v>
       </c>
@@ -14136,30 +13640,24 @@
       <c r="E76" s="100" t="s">
         <v>10</v>
       </c>
-      <c r="F76" s="99"/>
-      <c r="G76" s="99"/>
-      <c r="H76" s="99"/>
-      <c r="I76" s="99"/>
-      <c r="J76" s="99"/>
-      <c r="K76" s="99"/>
-      <c r="L76" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C76,CostProjections!$L$11:$L$92,0),MATCH(L$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="F76" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C76,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1697.4360739182023</v>
       </c>
-      <c r="M76" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C76,CostProjections!$L$11:$L$92,0),MATCH(M$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="G76" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C76,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>905.28555390345696</v>
       </c>
-      <c r="N76" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C76,CostProjections!$L$11:$L$92,0),MATCH(N$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="H76" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C76,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>850.15598491574201</v>
       </c>
-      <c r="O76" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C76,CostProjections!$L$11:$L$92,0),MATCH(O$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="I76" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C76,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>795.02641592803116</v>
       </c>
     </row>
-    <row r="77" spans="1:15" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B77" s="100" t="s">
         <v>141</v>
       </c>
@@ -14172,30 +13670,24 @@
       <c r="E77" s="100" t="s">
         <v>10</v>
       </c>
-      <c r="F77" s="99"/>
-      <c r="G77" s="99"/>
-      <c r="H77" s="99"/>
-      <c r="I77" s="99"/>
-      <c r="J77" s="99"/>
-      <c r="K77" s="99"/>
-      <c r="L77" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C77,CostProjections!$L$11:$L$92,0),MATCH(L$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="F77" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C77,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1697.4360739182023</v>
       </c>
-      <c r="M77" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C77,CostProjections!$L$11:$L$92,0),MATCH(M$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="G77" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C77,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>905.28555390345696</v>
       </c>
-      <c r="N77" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C77,CostProjections!$L$11:$L$92,0),MATCH(N$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="H77" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C77,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>850.15598491574201</v>
       </c>
-      <c r="O77" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C77,CostProjections!$L$11:$L$92,0),MATCH(O$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="I77" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C77,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>795.02641592803116</v>
       </c>
     </row>
-    <row r="78" spans="1:15" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B78" s="100" t="s">
         <v>142</v>
       </c>
@@ -14208,30 +13700,24 @@
       <c r="E78" s="100" t="s">
         <v>10</v>
       </c>
-      <c r="F78" s="99"/>
-      <c r="G78" s="99"/>
-      <c r="H78" s="99"/>
-      <c r="I78" s="99"/>
-      <c r="J78" s="99"/>
-      <c r="K78" s="99"/>
-      <c r="L78" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C78,CostProjections!$L$11:$L$92,0),MATCH(L$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="F78" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C78,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>2645.9522057126255</v>
       </c>
-      <c r="M78" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C78,CostProjections!$L$11:$L$92,0),MATCH(M$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="G78" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C78,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1411.1531768153391</v>
       </c>
-      <c r="N78" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C78,CostProjections!$L$11:$L$92,0),MATCH(N$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="H78" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C78,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1325.217566688757</v>
       </c>
-      <c r="O78" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C78,CostProjections!$L$11:$L$92,0),MATCH(O$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="I78" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C78,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1239.2819565621814</v>
       </c>
     </row>
-    <row r="79" spans="1:15" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B79" s="100" t="s">
         <v>143</v>
       </c>
@@ -14244,30 +13730,24 @@
       <c r="E79" s="100" t="s">
         <v>10</v>
       </c>
-      <c r="F79" s="99"/>
-      <c r="G79" s="99"/>
-      <c r="H79" s="99"/>
-      <c r="I79" s="99"/>
-      <c r="J79" s="99"/>
-      <c r="K79" s="99"/>
-      <c r="L79" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C79,CostProjections!$L$11:$L$92,0),MATCH(L$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="F79" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C79,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>2693.0881275829665</v>
       </c>
-      <c r="M79" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C79,CostProjections!$L$11:$L$92,0),MATCH(M$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="G79" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C79,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1436.2919551144494</v>
       </c>
-      <c r="N79" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C79,CostProjections!$L$11:$L$92,0),MATCH(N$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="H79" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C79,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1348.8254578478573</v>
       </c>
-      <c r="O79" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C79,CostProjections!$L$11:$L$92,0),MATCH(O$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="I79" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C79,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1261.3589605812717</v>
       </c>
     </row>
-    <row r="80" spans="1:15" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B80" s="100" t="s">
         <v>144</v>
       </c>
@@ -14280,30 +13760,24 @@
       <c r="E80" s="100" t="s">
         <v>10</v>
       </c>
-      <c r="F80" s="99"/>
-      <c r="G80" s="99"/>
-      <c r="H80" s="99"/>
-      <c r="I80" s="99"/>
-      <c r="J80" s="99"/>
-      <c r="K80" s="99"/>
-      <c r="L80" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C80,CostProjections!$L$11:$L$92,0),MATCH(L$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="F80" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C80,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>2693.0881275829665</v>
       </c>
-      <c r="M80" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C80,CostProjections!$L$11:$L$92,0),MATCH(M$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="G80" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C80,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1436.2919551144494</v>
       </c>
-      <c r="N80" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C80,CostProjections!$L$11:$L$92,0),MATCH(N$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="H80" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C80,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1348.8254578478573</v>
       </c>
-      <c r="O80" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C80,CostProjections!$L$11:$L$92,0),MATCH(O$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="I80" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C80,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1261.3589605812717</v>
       </c>
     </row>
-    <row r="81" spans="2:15" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:9" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B81" s="100" t="s">
         <v>145</v>
       </c>
@@ -14316,30 +13790,24 @@
       <c r="E81" s="100" t="s">
         <v>10</v>
       </c>
-      <c r="F81" s="99"/>
-      <c r="G81" s="99"/>
-      <c r="H81" s="99"/>
-      <c r="I81" s="99"/>
-      <c r="J81" s="99"/>
-      <c r="K81" s="99"/>
-      <c r="L81" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C81,CostProjections!$L$11:$L$92,0),MATCH(L$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="F81" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C81,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>3660.6104342648114</v>
       </c>
-      <c r="M81" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C81,CostProjections!$L$11:$L$92,0),MATCH(M$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="G81" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C81,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1952.2960513963292</v>
       </c>
-      <c r="N81" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C81,CostProjections!$L$11:$L$92,0),MATCH(N$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="H81" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C81,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1833.4062277535943</v>
       </c>
-      <c r="O81" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C81,CostProjections!$L$11:$L$92,0),MATCH(O$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="I81" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C81,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1714.5164041108685</v>
       </c>
     </row>
-    <row r="82" spans="2:15" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:9" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B82" s="100" t="s">
         <v>146</v>
       </c>
@@ -14352,30 +13820,24 @@
       <c r="E82" s="100" t="s">
         <v>10</v>
       </c>
-      <c r="F82" s="99"/>
-      <c r="G82" s="99"/>
-      <c r="H82" s="99"/>
-      <c r="I82" s="99"/>
-      <c r="J82" s="99"/>
-      <c r="K82" s="99"/>
-      <c r="L82" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C82,CostProjections!$L$11:$L$92,0),MATCH(L$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="F82" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C82,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>3660.6104342648114</v>
       </c>
-      <c r="M82" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C82,CostProjections!$L$11:$L$92,0),MATCH(M$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="G82" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C82,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1952.2960513963292</v>
       </c>
-      <c r="N82" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C82,CostProjections!$L$11:$L$92,0),MATCH(N$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="H82" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C82,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1833.4062277535943</v>
       </c>
-      <c r="O82" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C82,CostProjections!$L$11:$L$92,0),MATCH(O$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="I82" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C82,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1714.5164041108685</v>
       </c>
     </row>
-    <row r="83" spans="2:15" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:9" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B83" s="100" t="s">
         <v>147</v>
       </c>
@@ -14388,30 +13850,24 @@
       <c r="E83" s="100" t="s">
         <v>10</v>
       </c>
-      <c r="F83" s="99"/>
-      <c r="G83" s="99"/>
-      <c r="H83" s="99"/>
-      <c r="I83" s="99"/>
-      <c r="J83" s="99"/>
-      <c r="K83" s="99"/>
-      <c r="L83" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C83,CostProjections!$L$11:$L$92,0),MATCH(L$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="F83" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C83,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>3660.6104342648114</v>
       </c>
-      <c r="M83" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C83,CostProjections!$L$11:$L$92,0),MATCH(M$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="G83" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C83,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1952.2960513963292</v>
       </c>
-      <c r="N83" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C83,CostProjections!$L$11:$L$92,0),MATCH(N$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="H83" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C83,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1833.4062277535943</v>
       </c>
-      <c r="O83" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C83,CostProjections!$L$11:$L$92,0),MATCH(O$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+      <c r="I83" s="99">
+        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C83,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
         <v>1714.5164041108685</v>
       </c>
     </row>
-    <row r="84" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="84" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B84" s="16"/>
       <c r="C84" s="6"/>
       <c r="D84" s="6"/>
@@ -14420,25 +13876,13 @@
       <c r="G84" s="28"/>
       <c r="H84" s="28"/>
       <c r="I84" s="28"/>
-      <c r="J84" s="28"/>
-      <c r="K84" s="28"/>
-      <c r="L84" s="28"/>
-      <c r="M84" s="28"/>
-      <c r="N84" s="28"/>
-      <c r="O84" s="28"/>
-    </row>
-    <row r="85" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="F85" s="1"/>
-    </row>
-    <row r="86" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="F86" s="1"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="L8:O83">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+  <conditionalFormatting sqref="F8:I83">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="2">
+    <cfRule type="expression" dxfId="0" priority="2">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23253,7 +22697,7 @@
         <v>F</v>
       </c>
       <c r="J75" s="71" t="str">
-        <f t="shared" ref="J75:J106" si="31">IF(I75="P",IF(OR(C75="CAR",C75="SUV",C75="MOT"),"PR","PU"),C75)</f>
+        <f t="shared" ref="J75:J92" si="31">IF(I75="P",IF(OR(C75="CAR",C75="SUV",C75="MOT"),"PR","PU"),C75)</f>
         <v>HCV5</v>
       </c>
       <c r="K75" s="71" t="str">
@@ -23261,7 +22705,7 @@
         <v/>
       </c>
       <c r="L75" s="74" t="str">
-        <f t="shared" ref="L75:L106" si="33">H75&amp;I75&amp;J75&amp;K75&amp;A75&amp;"-N"</f>
+        <f t="shared" ref="L75:L92" si="33">H75&amp;I75&amp;J75&amp;K75&amp;A75&amp;"-N"</f>
         <v>TFHCV5HGN-N</v>
       </c>
       <c r="M75" s="74" t="str">

</xml_diff>

<commit_message>
Fixed FOM in IEA vehicle cost projection scenario
</commit_message>
<xml_diff>
--- a/suppxls/Scen_IEAcosts_TRA.xlsx
+++ b/suppxls/Scen_IEAcosts_TRA.xlsx
@@ -8,10 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SATIMGE_Veda\suppxls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{899A7558-5E40-4C2B-BFED-E283E4ECFEA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E157AAE5-59BD-4BDF-971E-39678F9B9AD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="735" yWindow="735" windowWidth="28800" windowHeight="15480" activeTab="1" xr2:uid="{E2E76818-39F4-4BBE-93AA-8C71FE1D5983}"/>
-    <workbookView xWindow="1080" yWindow="1080" windowWidth="28800" windowHeight="15480" activeTab="2" xr2:uid="{2CAB5348-3A5C-453D-8E79-FBBD2C206FCF}"/>
+    <workbookView xWindow="30" yWindow="390" windowWidth="28770" windowHeight="15570" activeTab="2" xr2:uid="{2CAB5348-3A5C-453D-8E79-FBBD2C206FCF}"/>
   </bookViews>
   <sheets>
     <sheet name="INVCOST" sheetId="13" r:id="rId1"/>
@@ -7767,10 +7766,7 @@
   </sheetPr>
   <dimension ref="A1:O86"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
-    </sheetView>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="1">
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
@@ -11321,10 +11317,7 @@
   </sheetPr>
   <dimension ref="A1:I84"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Q13" sqref="Q13"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -11481,20 +11474,20 @@
         <v>13</v>
       </c>
       <c r="F8" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C8,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>835.64408109927854</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C8,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>22.562390189680517</v>
       </c>
       <c r="G8" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C8,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>852.50818368869375</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C8,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>23.01772095959473</v>
       </c>
       <c r="H8" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C8,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>869.71262011470128</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C8,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>23.482240743096934</v>
       </c>
       <c r="I8" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C8,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>887.26425864199052</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C8,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>23.956134983333744</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -11514,20 +11507,20 @@
         <v>21</v>
       </c>
       <c r="F9" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C9,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>438.90146207526243</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C9,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>11.850339476032087</v>
       </c>
       <c r="G9" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C9,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>447.75891640359885</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C9,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>12.089490742897169</v>
       </c>
       <c r="H9" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C9,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>456.79512269326983</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C9,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>12.333468312718285</v>
       </c>
       <c r="I9" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C9,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>466.01368833105909</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C9,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>12.582369584938595</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -11544,20 +11537,20 @@
         <v>13</v>
       </c>
       <c r="F10" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C10,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1115.3529863163551</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C10,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>30.114530630541591</v>
       </c>
       <c r="G10" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C10,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>849.11877209576846</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C10,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>22.92620684658575</v>
       </c>
       <c r="H10" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C10,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>851.93042365899805</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C10,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>23.002121438792948</v>
       </c>
       <c r="I10" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C10,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>854.742075222229</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C10,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>23.078036031000181</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -11574,20 +11567,20 @@
         <v>21</v>
       </c>
       <c r="F11" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C11,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>585.81167209404305</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C11,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>15.816915146539161</v>
       </c>
       <c r="G11" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C11,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>445.97871148459467</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C11,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>12.041425210084057</v>
       </c>
       <c r="H11" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C11,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>447.45546218487397</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C11,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>12.081297478991596</v>
       </c>
       <c r="I11" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C11,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>448.93221288515406</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C11,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>12.12116974789916</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
@@ -11607,20 +11600,20 @@
         <v>12</v>
       </c>
       <c r="F12" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C12,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>919.2084892092065</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C12,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>24.818629208648577</v>
       </c>
       <c r="G12" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C12,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>937.75900205756318</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C12,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>25.319493055554204</v>
       </c>
       <c r="H12" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C12,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>956.68388212617151</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C12,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>25.830464817406632</v>
       </c>
       <c r="I12" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C12,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>975.99068450618972</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C12,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>26.351748481667119</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
@@ -11637,20 +11630,20 @@
         <v>10</v>
       </c>
       <c r="F13" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C13,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>3873.0540520727282</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C13,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>104.57245940596366</v>
       </c>
       <c r="G13" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C13,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>2065.5976014079038</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C13,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>55.771135238013407</v>
       </c>
       <c r="H13" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C13,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1939.8080038862586</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C13,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>52.374816104928982</v>
       </c>
       <c r="I13" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C13,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1814.0184063646227</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C13,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>48.978496971844812</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
@@ -11670,20 +11663,20 @@
         <v>11</v>
       </c>
       <c r="F14" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C14,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>438.90146207526243</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C14,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>11.850339476032087</v>
       </c>
       <c r="G14" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C14,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>447.75891640359885</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C14,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>12.089490742897169</v>
       </c>
       <c r="H14" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C14,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>456.79512269326983</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C14,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>12.333468312718285</v>
       </c>
       <c r="I14" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C14,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>466.01368833105909</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C14,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>12.582369584938595</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
@@ -11700,20 +11693,20 @@
         <v>9</v>
       </c>
       <c r="F15" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C15,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1516.7538557832556</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C15,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>30.714265579610924</v>
       </c>
       <c r="G15" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C15,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>808.92316097561422</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C15,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>16.380694009756191</v>
       </c>
       <c r="H15" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C15,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>759.66181463414648</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C15,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>15.383151746341468</v>
       </c>
       <c r="I15" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C15,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>710.40046829268272</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C15,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>14.385609482926824</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
@@ -11733,20 +11726,20 @@
         <v>13</v>
       </c>
       <c r="F16" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C16,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>656.10237784381934</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C16,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>17.714764201783122</v>
       </c>
       <c r="G16" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C16,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>669.34315589679386</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C16,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>18.072265209213434</v>
       </c>
       <c r="H16" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C16,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>682.85114560662009</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C16,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>18.436980931378745</v>
       </c>
       <c r="I16" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C16,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>696.63173956195692</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C16,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>18.80905696817284</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
@@ -11766,20 +11759,20 @@
         <v>21</v>
       </c>
       <c r="F17" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C17,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>262.38470575580084</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C17,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>7.0843870554066228</v>
       </c>
       <c r="G17" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C17,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>267.67988189100242</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C17,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>7.2273568110570654</v>
       </c>
       <c r="H17" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C17,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>273.08191978181594</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C17,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>7.3732118341090311</v>
       </c>
       <c r="I17" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C17,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>278.59297600141696</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C17,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>7.522010352038258</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
@@ -11796,20 +11789,20 @@
         <v>13</v>
       </c>
       <c r="F18" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C18,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1413.7180946041472</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C18,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>38.17038855431197</v>
       </c>
       <c r="G18" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C18,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1076.264274455765</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C18,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>29.059135410305654</v>
       </c>
       <c r="H18" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C18,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1079.8280634440273</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C18,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>29.155357712988735</v>
       </c>
       <c r="I18" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C18,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1083.3918524322912</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C18,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>29.251580015671866</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
@@ -11826,20 +11819,20 @@
         <v>21</v>
       </c>
       <c r="F19" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C19,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>565.36604469167128</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C19,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>15.264883206675124</v>
       </c>
       <c r="G19" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C19,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>430.41344537815206</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C19,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>11.621163025210105</v>
       </c>
       <c r="H19" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C19,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>431.83865546218487</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C19,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>11.659643697478991</v>
       </c>
       <c r="I19" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C19,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>433.26386554621848</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C19,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>11.698124369747898</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
@@ -11856,20 +11849,20 @@
         <v>9</v>
       </c>
       <c r="F20" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C20,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>996.58245713780525</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C20,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>20.180794757040555</v>
       </c>
       <c r="G20" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C20,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>531.50260889526839</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C20,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>10.762927830129186</v>
       </c>
       <c r="H20" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C20,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>499.13546284074624</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C20,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>10.107493122525112</v>
       </c>
       <c r="I20" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C20,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>466.76831678622648</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C20,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>9.4520584149210869</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
@@ -11889,20 +11882,20 @@
         <v>12</v>
       </c>
       <c r="F21" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C21,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>721.71261562820132</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C21,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>19.486240621961436</v>
       </c>
       <c r="G21" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C21,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>736.27747148647325</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C21,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>19.879491730134777</v>
       </c>
       <c r="H21" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C21,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>751.13626016728222</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C21,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>20.280679024516619</v>
       </c>
       <c r="I21" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C21,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>766.29491351815273</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C21,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>20.689962664990123</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
@@ -11919,20 +11912,20 @@
         <v>10</v>
       </c>
       <c r="F22" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C22,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>2544.7884698792823</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C22,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>68.709288686740621</v>
       </c>
       <c r="G22" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C22,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1357.2000000000075</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C22,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>36.644400000000196</v>
       </c>
       <c r="H22" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C22,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1274.5500000000002</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C22,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>34.412850000000006</v>
       </c>
       <c r="I22" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C22,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1191.8999999999996</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C22,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>32.181299999999986</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
@@ -11952,20 +11945,20 @@
         <v>11</v>
       </c>
       <c r="F23" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C23,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>262.38470575580084</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C23,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>7.0843870554066228</v>
       </c>
       <c r="G23" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C23,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>267.67988189100242</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C23,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>7.2273568110570654</v>
       </c>
       <c r="H23" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C23,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>273.08191978181594</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C23,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>7.3732118341090311</v>
       </c>
       <c r="I23" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C23,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>278.59297600141696</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C23,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>7.522010352038258</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
@@ -11985,20 +11978,20 @@
         <v>21</v>
       </c>
       <c r="F24" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C24,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>140.61345431714946</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C24,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>3.7965632665630351</v>
       </c>
       <c r="G24" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C24,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>143.45116928778262</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C24,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>3.8731815707701309</v>
       </c>
       <c r="H24" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C24,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>146.34615208028723</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C24,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>3.9513461061677551</v>
       </c>
       <c r="I24" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C24,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>149.29955841447855</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C24,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>4.0310880771909208</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
@@ -12015,20 +12008,20 @@
         <v>9</v>
       </c>
       <c r="F25" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C25,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>201.43776538895028</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C25,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>4.0791147491262434</v>
       </c>
       <c r="G25" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C25,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>107.43185078909673</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C25,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>2.1754949784792088</v>
       </c>
       <c r="H25" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C25,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>100.88952654232429</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C25,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>2.0430129124820668</v>
       </c>
       <c r="I25" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C25,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>94.347202295552336</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C25,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>1.9105308464849349</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
@@ -12048,20 +12041,20 @@
         <v>13</v>
       </c>
       <c r="F26" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C26,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1674.9173571001118</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C26,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>45.222768641703013</v>
       </c>
       <c r="G26" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C26,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1708.7188029283056</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C26,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>46.135407679064251</v>
       </c>
       <c r="H26" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C26,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1743.2023944965467</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C26,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>47.066464651406761</v>
       </c>
       <c r="I26" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C26,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1778.3818981630261</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C26,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>48.016311250401699</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
@@ -12081,20 +12074,20 @@
         <v>12</v>
       </c>
       <c r="F27" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C27,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1775.901197692195</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C27,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>47.94933233768927</v>
       </c>
       <c r="G27" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C27,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1811.7405947081456</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C27,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>48.916996057119931</v>
       </c>
       <c r="H27" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C27,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1848.303265282409</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C27,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>49.90418816262504</v>
       </c>
       <c r="I27" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C27,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1885.603805772171</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C27,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>50.911302755848617</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
@@ -12111,20 +12104,20 @@
         <v>10</v>
       </c>
       <c r="F28" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C28,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>3448.5361583131421</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C28,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>93.11047627445484</v>
       </c>
       <c r="G28" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C28,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1839.1914807302808</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C28,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>49.658169979717584</v>
       </c>
       <c r="H28" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C28,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1727.1894354293891</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C28,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>46.634114756593505</v>
       </c>
       <c r="I28" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C28,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1615.1873901285062</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C28,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>43.610059533469666</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
@@ -12144,20 +12137,20 @@
         <v>11</v>
       </c>
       <c r="F29" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C29,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1674.9173571001118</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C29,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>45.222768641703013</v>
       </c>
       <c r="G29" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C29,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1708.7188029283056</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C29,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>46.135407679064251</v>
       </c>
       <c r="H29" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C29,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1743.2023944965467</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C29,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>47.066464651406761</v>
       </c>
       <c r="I29" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C29,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1778.3818981630261</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C29,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>48.016311250401699</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
@@ -12174,20 +12167,20 @@
         <v>9</v>
       </c>
       <c r="F30" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C30,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>2885.1124291966107</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C30,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>58.423526691231366</v>
       </c>
       <c r="G30" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C30,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1538.7033677857753</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C30,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>31.158743197661952</v>
       </c>
       <c r="H30" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C30,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1445.0002780808647</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C30,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>29.261255631137512</v>
       </c>
       <c r="I30" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C30,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1351.2971883759612</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C30,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>27.363768064613218</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
@@ -12207,20 +12200,20 @@
         <v>13</v>
       </c>
       <c r="F31" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C31,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>835.64408109927854</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C31,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>22.562390189680517</v>
       </c>
       <c r="G31" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C31,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>852.50818368869375</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C31,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>23.01772095959473</v>
       </c>
       <c r="H31" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C31,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>869.71262011470128</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C31,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>23.482240743096934</v>
       </c>
       <c r="I31" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C31,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>887.26425864199052</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C31,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>23.956134983333744</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
@@ -12240,20 +12233,20 @@
         <v>21</v>
       </c>
       <c r="F32" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C32,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>438.90146207526243</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C32,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>11.850339476032087</v>
       </c>
       <c r="G32" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C32,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>447.75891640359885</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C32,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>12.089490742897169</v>
       </c>
       <c r="H32" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C32,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>456.79512269326983</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C32,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>12.333468312718285</v>
       </c>
       <c r="I32" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C32,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>466.01368833105909</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C32,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>12.582369584938595</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
@@ -12273,20 +12266,20 @@
         <v>12</v>
       </c>
       <c r="F33" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C33,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>919.2084892092065</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C33,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>24.818629208648577</v>
       </c>
       <c r="G33" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C33,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>937.75900205756318</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C33,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>25.319493055554204</v>
       </c>
       <c r="H33" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C33,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>956.68388212617151</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C33,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>25.830464817406632</v>
       </c>
       <c r="I33" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C33,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>975.99068450618972</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C33,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>26.351748481667119</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
@@ -12303,20 +12296,20 @@
         <v>10</v>
       </c>
       <c r="F34" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C34,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>3873.0540520727282</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C34,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>104.57245940596366</v>
       </c>
       <c r="G34" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C34,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>2065.5976014079038</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C34,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>55.771135238013407</v>
       </c>
       <c r="H34" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C34,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1939.8080038862586</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C34,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>52.374816104928982</v>
       </c>
       <c r="I34" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C34,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1814.0184063646227</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C34,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>48.978496971844812</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
@@ -12336,20 +12329,20 @@
         <v>11</v>
       </c>
       <c r="F35" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C35,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>438.90146207526243</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C35,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>11.850339476032087</v>
       </c>
       <c r="G35" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C35,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>447.75891640359885</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C35,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>12.089490742897169</v>
       </c>
       <c r="H35" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C35,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>456.79512269326983</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C35,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>12.333468312718285</v>
       </c>
       <c r="I35" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C35,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>466.01368833105909</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C35,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>12.582369584938595</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
@@ -12366,20 +12359,20 @@
         <v>9</v>
       </c>
       <c r="F36" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C36,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1516.7538557832556</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C36,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>30.714265579610924</v>
       </c>
       <c r="G36" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C36,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>808.92316097561422</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C36,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>16.380694009756191</v>
       </c>
       <c r="H36" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C36,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>759.66181463414648</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C36,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>15.383151746341468</v>
       </c>
       <c r="I36" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C36,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>710.40046829268272</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C36,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>14.385609482926824</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
@@ -12399,20 +12392,20 @@
         <v>13</v>
       </c>
       <c r="F37" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C37,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1674.9173571001118</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C37,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>45.222768641703013</v>
       </c>
       <c r="G37" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C37,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1708.7188029283056</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C37,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>46.135407679064251</v>
       </c>
       <c r="H37" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C37,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1743.2023944965467</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C37,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>47.066464651406761</v>
       </c>
       <c r="I37" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C37,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1778.3818981630261</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C37,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>48.016311250401699</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
@@ -12432,20 +12425,20 @@
         <v>12</v>
       </c>
       <c r="F38" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C38,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1775.901197692195</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C38,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>47.94933233768927</v>
       </c>
       <c r="G38" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C38,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1811.7405947081456</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C38,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>48.916996057119931</v>
       </c>
       <c r="H38" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C38,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1848.303265282409</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C38,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>49.90418816262504</v>
       </c>
       <c r="I38" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C38,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1885.603805772171</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C38,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>50.911302755848617</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
@@ -12462,20 +12455,20 @@
         <v>9</v>
       </c>
       <c r="F39" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C39,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>2885.1124291966107</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C39,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>58.423526691231366</v>
       </c>
       <c r="G39" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C39,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1538.7033677857753</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C39,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>31.158743197661952</v>
       </c>
       <c r="H39" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C39,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1445.0002780808647</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C39,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>29.261255631137512</v>
       </c>
       <c r="I39" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C39,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1351.2971883759612</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C39,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>27.363768064613218</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
@@ -12492,20 +12485,20 @@
         <v>10</v>
       </c>
       <c r="F40" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C40,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>3448.5361583131421</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C40,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>93.11047627445484</v>
       </c>
       <c r="G40" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C40,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1839.1914807302808</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C40,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>49.658169979717584</v>
       </c>
       <c r="H40" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C40,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1727.1894354293891</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C40,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>46.634114756593505</v>
       </c>
       <c r="I40" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C40,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1615.1873901285062</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C40,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>43.610059533469666</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
@@ -12525,20 +12518,20 @@
         <v>11</v>
       </c>
       <c r="F41" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C41,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1674.9173571001118</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C41,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>45.222768641703013</v>
       </c>
       <c r="G41" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C41,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1708.7188029283056</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C41,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>46.135407679064251</v>
       </c>
       <c r="H41" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C41,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1743.2023944965467</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C41,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>47.066464651406761</v>
       </c>
       <c r="I41" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C41,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1778.3818981630261</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C41,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>48.016311250401699</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
@@ -12558,20 +12551,20 @@
         <v>13</v>
       </c>
       <c r="F42" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C42,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>835.64408109927854</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C42,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>22.562390189680517</v>
       </c>
       <c r="G42" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C42,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>852.50818368869375</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C42,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>23.01772095959473</v>
       </c>
       <c r="H42" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C42,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>869.71262011470128</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C42,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>23.482240743096934</v>
       </c>
       <c r="I42" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C42,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>887.26425864199052</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C42,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>23.956134983333744</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
@@ -12588,20 +12581,20 @@
         <v>13</v>
       </c>
       <c r="F43" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C43,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1115.3529863163551</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C43,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>30.114530630541591</v>
       </c>
       <c r="G43" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C43,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>849.11877209576846</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C43,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>22.92620684658575</v>
       </c>
       <c r="H43" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C43,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>851.93042365899805</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C43,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>23.002121438792948</v>
       </c>
       <c r="I43" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C43,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>854.742075222229</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C43,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>23.078036031000181</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
@@ -12621,20 +12614,20 @@
         <v>21</v>
       </c>
       <c r="F44" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C44,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>438.90146207526243</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C44,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>11.850339476032087</v>
       </c>
       <c r="G44" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C44,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>447.75891640359885</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C44,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>12.089490742897169</v>
       </c>
       <c r="H44" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C44,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>456.79512269326983</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C44,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>12.333468312718285</v>
       </c>
       <c r="I44" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C44,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>466.01368833105909</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C44,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>12.582369584938595</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
@@ -12651,20 +12644,20 @@
         <v>21</v>
       </c>
       <c r="F45" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C45,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>585.81167209404305</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C45,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>15.816915146539161</v>
       </c>
       <c r="G45" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C45,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>445.97871148459467</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C45,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>12.041425210084057</v>
       </c>
       <c r="H45" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C45,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>447.45546218487397</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C45,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>12.081297478991596</v>
       </c>
       <c r="I45" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C45,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>448.93221288515406</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C45,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>12.12116974789916</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
@@ -12684,20 +12677,20 @@
         <v>12</v>
       </c>
       <c r="F46" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C46,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>919.2084892092065</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C46,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>24.818629208648577</v>
       </c>
       <c r="G46" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C46,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>937.75900205756318</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C46,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>25.319493055554204</v>
       </c>
       <c r="H46" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C46,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>956.68388212617151</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C46,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>25.830464817406632</v>
       </c>
       <c r="I46" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C46,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>975.99068450618972</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C46,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>26.351748481667119</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
@@ -12714,20 +12707,20 @@
         <v>9</v>
       </c>
       <c r="F47" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C47,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1516.7538557832556</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C47,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>30.714265579610924</v>
       </c>
       <c r="G47" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C47,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>808.92316097561422</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C47,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>16.380694009756191</v>
       </c>
       <c r="H47" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C47,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>759.66181463414648</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C47,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>15.383151746341468</v>
       </c>
       <c r="I47" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C47,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>710.40046829268272</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C47,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>14.385609482926824</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
@@ -12747,20 +12740,20 @@
         <v>13</v>
       </c>
       <c r="F48" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C48,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>522.57584162425417</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C48,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>14.109547723854861</v>
       </c>
       <c r="G48" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C48,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>533.12192554111539</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C48,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>14.394291989610114</v>
       </c>
       <c r="H48" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C48,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>543.88083959117944</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C48,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>14.684782668961844</v>
       </c>
       <c r="I48" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C48,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>554.85687889156804</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C48,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>14.981135730072339</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
@@ -12780,20 +12773,20 @@
         <v>21</v>
       </c>
       <c r="F49" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C49,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>411.73058994760896</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C49,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>11.116725928585442</v>
       </c>
       <c r="G49" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C49,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>420.0397099008585</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C49,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>11.341072167323178</v>
       </c>
       <c r="H49" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C49,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>428.51651589950546</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C49,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>11.569945929286646</v>
       </c>
       <c r="I49" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C49,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>437.16439200948946</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C49,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>11.803438584256215</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
@@ -12813,20 +12806,20 @@
         <v>13</v>
       </c>
       <c r="F50" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C50,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>522.57584162425417</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C50,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>14.109547723854861</v>
       </c>
       <c r="G50" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C50,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>533.12192554111539</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C50,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>14.394291989610114</v>
       </c>
       <c r="H50" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C50,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>543.88083959117944</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C50,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>14.684782668961844</v>
       </c>
       <c r="I50" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C50,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>554.85687889156804</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C50,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>14.981135730072339</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.2">
@@ -12846,20 +12839,20 @@
         <v>13</v>
       </c>
       <c r="F51" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C51,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>522.57584162425417</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C51,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>14.109547723854861</v>
       </c>
       <c r="G51" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C51,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>533.12192554111539</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C51,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>14.394291989610114</v>
       </c>
       <c r="H51" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C51,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>543.88083959117944</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C51,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>14.684782668961844</v>
       </c>
       <c r="I51" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C51,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>554.85687889156804</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C51,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>14.981135730072339</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">
@@ -12879,20 +12872,20 @@
         <v>13</v>
       </c>
       <c r="F52" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C52,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>902.73536260054868</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C52,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>24.373854790214814</v>
       </c>
       <c r="G52" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C52,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>920.95343188425818</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C52,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>24.865742660874972</v>
       </c>
       <c r="H52" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C52,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>939.53915935681937</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C52,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>25.367557302634122</v>
       </c>
       <c r="I52" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C52,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>958.49996471467352</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C52,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>25.879499047296186</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
@@ -12912,20 +12905,20 @@
         <v>13</v>
       </c>
       <c r="F53" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C53,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>858.22359532891846</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C53,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>23.172037073880798</v>
       </c>
       <c r="G53" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C53,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>875.54337426787095</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C53,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>23.639671105232516</v>
       </c>
       <c r="H53" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C53,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>893.21268303113357</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C53,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>24.116742441840604</v>
       </c>
       <c r="I53" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C53,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>911.23857546728675</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C53,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>24.603441537616742</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.2">
@@ -12945,20 +12938,20 @@
         <v>13</v>
       </c>
       <c r="F54" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C54,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>858.22359532891846</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C54,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>23.172037073880798</v>
       </c>
       <c r="G54" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C54,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>875.54337426787095</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C54,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>23.639671105232516</v>
       </c>
       <c r="H54" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C54,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>893.21268303113357</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C54,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>24.116742441840604</v>
       </c>
       <c r="I54" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C54,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>911.23857546728675</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C54,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>24.603441537616742</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.2">
@@ -12978,20 +12971,20 @@
         <v>13</v>
       </c>
       <c r="F55" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C55,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1128.5294733678718</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C55,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>30.470295780932535</v>
       </c>
       <c r="G55" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C55,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1151.3042853297043</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C55,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>31.085215703902012</v>
       </c>
       <c r="H55" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C55,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1174.5387149374535</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C55,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>31.712545303311245</v>
       </c>
       <c r="I55" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C55,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1198.2420377179947</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C55,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>32.352535018385858</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.2">
@@ -13011,20 +13004,20 @@
         <v>13</v>
       </c>
       <c r="F56" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C56,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1128.5294733678718</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C56,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>30.470295780932535</v>
       </c>
       <c r="G56" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C56,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1151.3042853297043</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C56,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>31.085215703902012</v>
       </c>
       <c r="H56" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C56,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1174.5387149374535</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C56,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>31.712545303311245</v>
       </c>
       <c r="I56" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C56,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1198.2420377179947</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C56,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>32.352535018385858</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
@@ -13044,20 +13037,20 @@
         <v>13</v>
       </c>
       <c r="F57" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C57,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1128.5294733678718</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C57,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>30.470295780932535</v>
       </c>
       <c r="G57" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C57,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1151.3042853297043</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C57,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>31.085215703902012</v>
       </c>
       <c r="H57" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C57,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1174.5387149374535</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C57,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>31.712545303311245</v>
       </c>
       <c r="I57" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C57,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1198.2420377179947</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C57,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>32.352535018385858</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
@@ -13077,20 +13070,20 @@
         <v>12</v>
       </c>
       <c r="F58" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C58,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>645.6084743842323</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C58,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>17.431428808374271</v>
       </c>
       <c r="G58" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C58,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>658.63747535590073</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C58,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>17.783211834609318</v>
       </c>
       <c r="H58" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C58,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>671.92941411890092</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C58,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>18.142094181210322</v>
       </c>
       <c r="I58" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C58,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>685.48959701116814</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C58,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>18.50821911930154</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
@@ -13110,20 +13103,20 @@
         <v>12</v>
       </c>
       <c r="F59" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C59,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>645.6084743842323</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C59,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>17.431428808374271</v>
       </c>
       <c r="G59" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C59,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>658.63747535590073</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C59,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>17.783211834609318</v>
       </c>
       <c r="H59" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C59,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>671.92941411890092</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C59,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>18.142094181210322</v>
       </c>
       <c r="I59" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C59,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>685.48959701116814</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C59,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>18.50821911930154</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.2">
@@ -13143,20 +13136,20 @@
         <v>12</v>
       </c>
       <c r="F60" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C60,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>645.6084743842323</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C60,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>17.431428808374271</v>
       </c>
       <c r="G60" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C60,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>658.63747535590073</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C60,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>17.783211834609318</v>
       </c>
       <c r="H60" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C60,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>671.92941411890092</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C60,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>18.142094181210322</v>
       </c>
       <c r="I60" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C60,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>685.48959701116814</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C60,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>18.50821911930154</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.2">
@@ -13176,20 +13169,20 @@
         <v>12</v>
       </c>
       <c r="F61" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C61,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1086.2358398404897</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C61,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>29.328367675693222</v>
       </c>
       <c r="G61" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C61,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1108.1571255334031</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C61,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>29.920242389401885</v>
       </c>
       <c r="H61" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C61,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1130.5208038898666</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C61,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>30.524061705026394</v>
       </c>
       <c r="I61" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C61,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1153.3358028200171</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C61,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>31.14006667614046</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.2">
@@ -13209,20 +13202,20 @@
         <v>12</v>
       </c>
       <c r="F62" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C62,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>991.12866157757253</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C62,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>26.760473862594456</v>
       </c>
       <c r="G62" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C62,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1011.130592789921</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C62,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>27.300526005327868</v>
       </c>
       <c r="H62" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C62,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1031.5361822433565</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C62,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>27.851476920570626</v>
       </c>
       <c r="I62" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C62,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1052.3535761500559</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C62,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>28.413546556051511</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.2">
@@ -13242,20 +13235,20 @@
         <v>12</v>
       </c>
       <c r="F63" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C63,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>991.12866157757253</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C63,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>26.760473862594456</v>
       </c>
       <c r="G63" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C63,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1011.130592789921</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C63,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>27.300526005327868</v>
       </c>
       <c r="H63" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C63,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1031.5361822433565</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C63,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>27.851476920570626</v>
       </c>
       <c r="I63" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C63,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1052.3535761500559</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C63,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>28.413546556051511</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.2">
@@ -13275,20 +13268,20 @@
         <v>12</v>
       </c>
       <c r="F64" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C64,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1308.7827191732849</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C64,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>35.337133417678693</v>
       </c>
       <c r="G64" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C64,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1335.1952152856936</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C64,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>36.050270812713727</v>
       </c>
       <c r="H64" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C64,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1362.1407410146062</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C64,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>36.777800007394362</v>
       </c>
       <c r="I64" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C64,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1389.6300534111874</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C64,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>37.520011442102053</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.2">
@@ -13308,20 +13301,20 @@
         <v>12</v>
       </c>
       <c r="F65" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C65,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1308.7827191732849</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C65,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>35.337133417678693</v>
       </c>
       <c r="G65" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C65,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1335.1952152856936</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C65,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>36.050270812713727</v>
       </c>
       <c r="H65" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C65,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1362.1407410146062</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C65,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>36.777800007394362</v>
       </c>
       <c r="I65" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C65,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1389.6300534111874</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C65,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>37.520011442102053</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.2">
@@ -13341,20 +13334,20 @@
         <v>12</v>
       </c>
       <c r="F66" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C66,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1308.7827191732849</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C66,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>35.337133417678693</v>
       </c>
       <c r="G66" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C66,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1335.1952152856936</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C66,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>36.050270812713727</v>
       </c>
       <c r="H66" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C66,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1362.1407410146062</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C66,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>36.777800007394362</v>
       </c>
       <c r="I66" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C66,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1389.6300534111874</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C66,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>37.520011442102053</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.2">
@@ -13371,20 +13364,20 @@
         <v>9</v>
       </c>
       <c r="F67" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C67,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1161.917203295312</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C67,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>23.528823366730066</v>
       </c>
       <c r="G67" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C67,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>619.67980717360467</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C67,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>12.548516095265494</v>
       </c>
       <c r="H67" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C67,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>581.94289583931152</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C67,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>11.78434364074606</v>
       </c>
       <c r="I67" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C67,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>544.20598450502132</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C67,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>11.020171186226682</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.2">
@@ -13401,20 +13394,20 @@
         <v>9</v>
       </c>
       <c r="F68" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C68,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1161.917203295312</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C68,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>23.528823366730066</v>
       </c>
       <c r="G68" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C68,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>619.67980717360467</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C68,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>12.548516095265494</v>
       </c>
       <c r="H68" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C68,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>581.94289583931152</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C68,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>11.78434364074606</v>
       </c>
       <c r="I68" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C68,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>544.20598450502132</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C68,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>11.020171186226682</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.2">
@@ -13431,20 +13424,20 @@
         <v>9</v>
       </c>
       <c r="F69" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C69,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1161.917203295312</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C69,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>23.528823366730066</v>
       </c>
       <c r="G69" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C69,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>619.67980717360467</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C69,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>12.548516095265494</v>
       </c>
       <c r="H69" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C69,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>581.94289583931152</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C69,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>11.78434364074606</v>
       </c>
       <c r="I69" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C69,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>544.20598450502132</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C69,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>11.020171186226682</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.2">
@@ -13461,20 +13454,20 @@
         <v>9</v>
       </c>
       <c r="F70" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C70,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>2007.179942663324</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C70,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>40.645393838932314</v>
       </c>
       <c r="G70" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C70,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1070.4797866016361</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C70,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>21.677215678683133</v>
       </c>
       <c r="H70" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C70,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1005.2903124175569</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C70,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>20.357128826455526</v>
       </c>
       <c r="I70" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C70,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>940.10083823348259</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C70,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>19.037041974228021</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.2">
@@ -13491,20 +13484,20 @@
         <v>9</v>
       </c>
       <c r="F71" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C71,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1908.21059884285</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C71,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>38.641264626567711</v>
       </c>
       <c r="G71" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C71,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1017.6969345009586</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C71,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>20.60836292364441</v>
       </c>
       <c r="H71" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C71,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>955.72180066916428</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C71,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>19.353366463550579</v>
       </c>
       <c r="I71" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C71,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>893.74666683737496</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C71,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>18.098370003456843</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.2">
@@ -13521,20 +13514,20 @@
         <v>9</v>
       </c>
       <c r="F72" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C72,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1908.21059884285</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C72,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>38.641264626567711</v>
       </c>
       <c r="G72" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C72,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1017.6969345009586</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C72,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>20.60836292364441</v>
       </c>
       <c r="H72" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C72,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>955.72180066916428</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C72,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>19.353366463550579</v>
       </c>
       <c r="I72" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C72,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>893.74666683737496</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C72,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>18.098370003456843</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.2">
@@ -13551,20 +13544,20 @@
         <v>9</v>
       </c>
       <c r="F73" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C73,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>2509.2201075662383</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C73,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>50.811707178216324</v>
       </c>
       <c r="G73" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C73,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1338.2304935350739</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C73,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>27.09916749408525</v>
       </c>
       <c r="H73" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C73,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1256.7356878390212</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C73,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>25.448897678740181</v>
       </c>
       <c r="I73" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C73,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1175.2408821429744</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C73,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>23.798627863395236</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.2">
@@ -13581,20 +13574,20 @@
         <v>9</v>
       </c>
       <c r="F74" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C74,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>2509.2201075662383</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C74,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>50.811707178216324</v>
       </c>
       <c r="G74" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C74,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1338.2304935350739</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C74,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>27.09916749408525</v>
       </c>
       <c r="H74" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C74,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1256.7356878390212</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C74,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>25.448897678740181</v>
       </c>
       <c r="I74" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C74,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1175.2408821429744</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C74,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>23.798627863395236</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.2">
@@ -13611,20 +13604,20 @@
         <v>9</v>
       </c>
       <c r="F75" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C75,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>2509.2201075662383</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C75,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>50.811707178216324</v>
       </c>
       <c r="G75" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C75,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1338.2304935350739</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C75,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>27.09916749408525</v>
       </c>
       <c r="H75" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C75,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1256.7356878390212</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C75,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>25.448897678740181</v>
       </c>
       <c r="I75" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C75,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1175.2408821429744</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C75,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>23.798627863395236</v>
       </c>
     </row>
     <row r="76" spans="1:9" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -13641,20 +13634,20 @@
         <v>10</v>
       </c>
       <c r="F76" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C76,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1697.4360739182023</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C76,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>34.373080496843599</v>
       </c>
       <c r="G76" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C76,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>905.28555390345696</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C76,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>18.332032466545002</v>
       </c>
       <c r="H76" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C76,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>850.15598491574201</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C76,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>17.215658694543773</v>
       </c>
       <c r="I76" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C76,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>795.02641592803116</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C76,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>16.09928492254263</v>
       </c>
     </row>
     <row r="77" spans="1:9" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -13671,20 +13664,20 @@
         <v>10</v>
       </c>
       <c r="F77" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C77,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1697.4360739182023</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C77,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>34.373080496843599</v>
       </c>
       <c r="G77" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C77,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>905.28555390345696</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C77,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>18.332032466545002</v>
       </c>
       <c r="H77" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C77,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>850.15598491574201</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C77,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>17.215658694543773</v>
       </c>
       <c r="I77" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C77,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>795.02641592803116</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C77,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>16.09928492254263</v>
       </c>
     </row>
     <row r="78" spans="1:9" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -13701,20 +13694,20 @@
         <v>10</v>
       </c>
       <c r="F78" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C78,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>2645.9522057126255</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C78,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>53.580532165680665</v>
       </c>
       <c r="G78" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C78,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1411.1531768153391</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C78,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>28.575851830510619</v>
       </c>
       <c r="H78" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C78,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1325.217566688757</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C78,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>26.835655725447332</v>
       </c>
       <c r="I78" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C78,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1239.2819565621814</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C78,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>25.095459620384176</v>
       </c>
     </row>
     <row r="79" spans="1:9" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -13731,20 +13724,20 @@
         <v>10</v>
       </c>
       <c r="F79" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C79,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>2693.0881275829665</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C79,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>54.535034583555067</v>
       </c>
       <c r="G79" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C79,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1436.2919551144494</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C79,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>29.084912091067601</v>
       </c>
       <c r="H79" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C79,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1348.8254578478573</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C79,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>27.313715521419109</v>
       </c>
       <c r="I79" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C79,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1261.3589605812717</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C79,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>25.542518951770752</v>
       </c>
     </row>
     <row r="80" spans="1:9" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -13761,20 +13754,20 @@
         <v>10</v>
       </c>
       <c r="F80" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C80,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>2693.0881275829665</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C80,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>54.535034583555067</v>
       </c>
       <c r="G80" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C80,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1436.2919551144494</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C80,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>29.084912091067601</v>
       </c>
       <c r="H80" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C80,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1348.8254578478573</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C80,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>27.313715521419109</v>
       </c>
       <c r="I80" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C80,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1261.3589605812717</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C80,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>25.542518951770752</v>
       </c>
     </row>
     <row r="81" spans="2:9" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -13791,20 +13784,20 @@
         <v>10</v>
       </c>
       <c r="F81" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C81,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>3660.6104342648114</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C81,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>74.127361293862435</v>
       </c>
       <c r="G81" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C81,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1952.2960513963292</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C81,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>39.533995040775672</v>
       </c>
       <c r="H81" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C81,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1833.4062277535943</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C81,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>37.126476112010288</v>
       </c>
       <c r="I81" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C81,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1714.5164041108685</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C81,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>34.718957183245088</v>
       </c>
     </row>
     <row r="82" spans="2:9" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -13821,20 +13814,20 @@
         <v>10</v>
       </c>
       <c r="F82" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C82,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>3660.6104342648114</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C82,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>74.127361293862435</v>
       </c>
       <c r="G82" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C82,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1952.2960513963292</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C82,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>39.533995040775672</v>
       </c>
       <c r="H82" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C82,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1833.4062277535943</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C82,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>37.126476112010288</v>
       </c>
       <c r="I82" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C82,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1714.5164041108685</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C82,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>34.718957183245088</v>
       </c>
     </row>
     <row r="83" spans="2:9" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -13851,20 +13844,20 @@
         <v>10</v>
       </c>
       <c r="F83" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C83,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>3660.6104342648114</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C83,CostProjections!$L$11:$L$92,0),MATCH(F$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>74.127361293862435</v>
       </c>
       <c r="G83" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C83,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1952.2960513963292</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C83,CostProjections!$L$11:$L$92,0),MATCH(G$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>39.533995040775672</v>
       </c>
       <c r="H83" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C83,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1833.4062277535943</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C83,CostProjections!$L$11:$L$92,0),MATCH(H$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>37.126476112010288</v>
       </c>
       <c r="I83" s="99">
-        <f>IFERROR(INDEX(CostProjections!$N$11:$W$92,MATCH($C83,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
-        <v>1714.5164041108685</v>
+        <f>IFERROR(INDEX(CostProjections!$Y$11:$AH$92,MATCH($C83,CostProjections!$L$11:$L$92,0),MATCH(I$6,CostProjections!$N$10:$W$10,0))*0.001,"")</f>
+        <v>34.718957183245088</v>
       </c>
     </row>
     <row r="84" spans="2:9" x14ac:dyDescent="0.2">
@@ -13898,10 +13891,7 @@
   </sheetPr>
   <dimension ref="A1:AH92"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
-    </sheetView>
-    <sheetView tabSelected="1" topLeftCell="Q35" workbookViewId="1">
+    <sheetView tabSelected="1" topLeftCell="Q35" workbookViewId="0">
       <selection activeCell="X35" sqref="X35"/>
     </sheetView>
   </sheetViews>
@@ -25034,10 +25024,7 @@
   </sheetPr>
   <dimension ref="A1:T131"/>
   <sheetViews>
-    <sheetView topLeftCell="G33" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
-    </sheetView>
-    <sheetView topLeftCell="A69" workbookViewId="1">
+    <sheetView topLeftCell="A69" workbookViewId="0">
       <selection activeCell="M4" sqref="M4:M5"/>
     </sheetView>
   </sheetViews>
@@ -27570,10 +27557,7 @@
   </sheetPr>
   <dimension ref="A2:AX19"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
-    </sheetView>
-    <sheetView workbookViewId="1">
+    <sheetView workbookViewId="0">
       <selection activeCell="M4" sqref="M4:M5"/>
     </sheetView>
   </sheetViews>

</xml_diff>